<commit_message>
Added in a mock example of what preferences might look like, cleaned up some of the old to do comments and fixed a typo that may have been messing with the allocations display.
</commit_message>
<xml_diff>
--- a/tas/public/template2.xlsx
+++ b/tas/public/template2.xlsx
@@ -16,77 +16,77 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="48">
   <si>
     <t>Code</t>
   </si>
   <si>
+    <t>CAB210</t>
+  </si>
+  <si>
+    <t>CAB220</t>
+  </si>
+  <si>
+    <t>CAB230</t>
+  </si>
+  <si>
+    <t>CAB240</t>
+  </si>
+  <si>
+    <t>CAB301</t>
+  </si>
+  <si>
+    <t>CAB302</t>
+  </si>
+  <si>
+    <t>CAB303</t>
+  </si>
+  <si>
+    <t>CAB202</t>
+  </si>
+  <si>
     <t>CAB201</t>
   </si>
   <si>
-    <t>CAB202</t>
-  </si>
-  <si>
     <t>CAB203</t>
   </si>
   <si>
-    <t>CAB210</t>
-  </si>
-  <si>
-    <t>CAB220</t>
-  </si>
-  <si>
-    <t>CAB230</t>
-  </si>
-  <si>
-    <t>CAB240</t>
-  </si>
-  <si>
-    <t>CAB301</t>
-  </si>
-  <si>
-    <t>CAB302</t>
-  </si>
-  <si>
-    <t>CAB303</t>
-  </si>
-  <si>
     <t>Standard Load:</t>
   </si>
   <si>
     <t>Name</t>
   </si>
   <si>
+    <t>People Context &amp; Tech</t>
+  </si>
+  <si>
+    <t>Fund of Data Science</t>
+  </si>
+  <si>
+    <t>Web Computing</t>
+  </si>
+  <si>
+    <t>Information Security</t>
+  </si>
+  <si>
+    <t>Algorithms &amp; Complexity</t>
+  </si>
+  <si>
+    <t>Software Development</t>
+  </si>
+  <si>
+    <t>Networks</t>
+  </si>
+  <si>
+    <t>Micro Proc and Dig Sys</t>
+  </si>
+  <si>
     <t>Programming Principles</t>
   </si>
   <si>
-    <t>Micro Proc and Dig Sys</t>
-  </si>
-  <si>
     <t>Discrete Structures</t>
   </si>
   <si>
-    <t>People Context &amp; Tech</t>
-  </si>
-  <si>
-    <t>Fund of Data Science</t>
-  </si>
-  <si>
-    <t>Web Computing</t>
-  </si>
-  <si>
-    <t>Information Security</t>
-  </si>
-  <si>
-    <t>Algorithms &amp; Complexity</t>
-  </si>
-  <si>
-    <t>Software Development</t>
-  </si>
-  <si>
-    <t>Networks</t>
-  </si>
-  <si>
     <t>Semester</t>
   </si>
   <si>
@@ -126,37 +126,37 @@
     <t>Load Error</t>
   </si>
   <si>
+    <t xml:space="preserve"> Kom Poota</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sergine Aldéric </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dennis Darren </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Timotha Lanny </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lorrie Sheila </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nia Kerena </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hellen Tatianna </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Avice Preston </t>
+  </si>
+  <si>
     <t xml:space="preserve"> Mantis Tobogan</t>
-  </si>
-  <si>
-    <t>CS</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t xml:space="preserve"> Dennis Darren </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Sergine Aldéric </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Kom Poota</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Lorrie Sheila </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Nia Kerena </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Timotha Lanny </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Hellen Tatianna </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Avice Preston </t>
   </si>
   <si>
     <t>9 Bodies</t>
@@ -569,34 +569,34 @@
         <v>1</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>10</v>
@@ -1299,34 +1299,34 @@
         <v>13</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="Q2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>22</v>
@@ -2020,7 +2020,7 @@
         <v>23</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I3">
         <v>2</v>
@@ -2035,25 +2035,25 @@
         <v>1</v>
       </c>
       <c r="M3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N3">
         <v>2</v>
       </c>
       <c r="O3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
         <v>2</v>
       </c>
-      <c r="Q3">
-        <v>1</v>
-      </c>
       <c r="R3">
         <v>1</v>
       </c>
       <c r="S3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" ht="17.45" customHeight="1" spans="7:19" x14ac:dyDescent="0.25">
@@ -2061,40 +2061,40 @@
         <v>24</v>
       </c>
       <c r="H4">
+        <v>180</v>
+      </c>
+      <c r="I4">
+        <v>50</v>
+      </c>
+      <c r="J4">
+        <v>400</v>
+      </c>
+      <c r="K4">
+        <v>550</v>
+      </c>
+      <c r="L4">
+        <v>500</v>
+      </c>
+      <c r="M4">
+        <v>600</v>
+      </c>
+      <c r="N4">
+        <v>630</v>
+      </c>
+      <c r="O4">
+        <v>670</v>
+      </c>
+      <c r="P4">
         <v>490</v>
       </c>
-      <c r="I4">
+      <c r="Q4">
         <v>610</v>
       </c>
-      <c r="J4">
+      <c r="R4">
         <v>610</v>
       </c>
-      <c r="K4">
-        <v>670</v>
-      </c>
-      <c r="L4">
+      <c r="S4">
         <v>680</v>
-      </c>
-      <c r="M4">
-        <v>180</v>
-      </c>
-      <c r="N4">
-        <v>50</v>
-      </c>
-      <c r="O4">
-        <v>400</v>
-      </c>
-      <c r="P4">
-        <v>550</v>
-      </c>
-      <c r="Q4">
-        <v>500</v>
-      </c>
-      <c r="R4">
-        <v>600</v>
-      </c>
-      <c r="S4">
-        <v>630</v>
       </c>
     </row>
     <row r="5" ht="18" customHeight="1" spans="7:19" x14ac:dyDescent="0.25">
@@ -2105,34 +2105,34 @@
         <v>1</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
         <v>0.6</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
-      <c r="N5">
-        <v>0.5</v>
-      </c>
-      <c r="O5">
-        <v>1</v>
-      </c>
-      <c r="P5">
-        <v>1</v>
-      </c>
-      <c r="Q5">
-        <v>1</v>
-      </c>
-      <c r="R5">
-        <v>1</v>
       </c>
       <c r="S5">
         <v>1</v>
@@ -2149,40 +2149,40 @@
         <v>27</v>
       </c>
       <c r="H6">
-        <v>1.845098</v>
+        <v>1.4101745</v>
       </c>
       <c r="I6">
-        <v>1.9402318</v>
+        <v>0.42693597</v>
       </c>
       <c r="J6">
-        <v>1.164139</v>
+        <v>1.756962</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>1.8952646</v>
       </c>
       <c r="L6">
-        <v>1.9874109</v>
+        <v>1.853872</v>
       </c>
       <c r="M6">
-        <v>1.4101745</v>
+        <v>1.9330533</v>
       </c>
       <c r="N6">
-        <v>0.42693597</v>
+        <v>1.9542425</v>
       </c>
       <c r="O6">
-        <v>1.756962</v>
+        <v>NaN</v>
       </c>
       <c r="P6">
-        <v>1.8952646</v>
+        <v>NaN</v>
       </c>
       <c r="Q6">
-        <v>1.853872</v>
+        <v>NaN</v>
       </c>
       <c r="R6">
-        <v>1.9330533</v>
+        <v>NaN</v>
       </c>
       <c r="S6">
-        <v>1.9542425</v>
+        <v>NaN</v>
       </c>
       <c r="T6" t="s">
         <v>28</v>
@@ -2307,11 +2307,11 @@
       <c r="G9">
         <f>F9-E9</f>
       </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
+      <c r="H9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I9" t="s">
+        <v>38</v>
       </c>
       <c r="J9" t="s">
         <v>38</v>
@@ -2331,11 +2331,11 @@
       <c r="O9" t="s">
         <v>38</v>
       </c>
-      <c r="P9" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>38</v>
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
       </c>
       <c r="R9" t="s">
         <v>38</v>
@@ -2375,8 +2375,8 @@
       <c r="K10" t="s">
         <v>38</v>
       </c>
-      <c r="L10">
-        <v>1</v>
+      <c r="L10" t="s">
+        <v>38</v>
       </c>
       <c r="M10" t="s">
         <v>38</v>
@@ -2384,8 +2384,8 @@
       <c r="N10" t="s">
         <v>38</v>
       </c>
-      <c r="O10" t="s">
-        <v>38</v>
+      <c r="O10">
+        <v>1</v>
       </c>
       <c r="P10" t="s">
         <v>38</v>
@@ -2393,8 +2393,8 @@
       <c r="Q10" t="s">
         <v>38</v>
       </c>
-      <c r="R10" t="s">
-        <v>38</v>
+      <c r="R10">
+        <v>1</v>
       </c>
       <c r="S10" t="s">
         <v>38</v>
@@ -2425,11 +2425,11 @@
       <c r="I11" t="s">
         <v>38</v>
       </c>
-      <c r="J11">
-        <v>1</v>
-      </c>
-      <c r="K11">
-        <v>1</v>
+      <c r="J11" t="s">
+        <v>38</v>
+      </c>
+      <c r="K11" t="s">
+        <v>38</v>
       </c>
       <c r="L11" t="s">
         <v>38</v>
@@ -2452,8 +2452,8 @@
       <c r="R11" t="s">
         <v>38</v>
       </c>
-      <c r="S11" t="s">
-        <v>38</v>
+      <c r="S11">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -2537,8 +2537,8 @@
       <c r="I13" t="s">
         <v>38</v>
       </c>
-      <c r="J13" t="s">
-        <v>38</v>
+      <c r="J13">
+        <v>1</v>
       </c>
       <c r="K13" t="s">
         <v>38</v>
@@ -2552,8 +2552,8 @@
       <c r="N13" t="s">
         <v>38</v>
       </c>
-      <c r="O13">
-        <v>1</v>
+      <c r="O13" t="s">
+        <v>38</v>
       </c>
       <c r="P13" t="s">
         <v>38</v>
@@ -2596,8 +2596,8 @@
       <c r="J14" t="s">
         <v>38</v>
       </c>
-      <c r="K14" t="s">
-        <v>38</v>
+      <c r="K14">
+        <v>1</v>
       </c>
       <c r="L14" t="s">
         <v>38</v>
@@ -2611,8 +2611,8 @@
       <c r="O14" t="s">
         <v>38</v>
       </c>
-      <c r="P14">
-        <v>1</v>
+      <c r="P14" t="s">
+        <v>38</v>
       </c>
       <c r="Q14" t="s">
         <v>38</v>
@@ -2661,8 +2661,8 @@
       <c r="M15">
         <v>1</v>
       </c>
-      <c r="N15">
-        <v>1</v>
+      <c r="N15" t="s">
+        <v>38</v>
       </c>
       <c r="O15" t="s">
         <v>38</v>
@@ -2729,8 +2729,8 @@
       <c r="Q16" t="s">
         <v>38</v>
       </c>
-      <c r="R16">
-        <v>1</v>
+      <c r="R16" t="s">
+        <v>38</v>
       </c>
       <c r="S16" t="s">
         <v>38</v>
@@ -2779,8 +2779,8 @@
       <c r="O17" t="s">
         <v>38</v>
       </c>
-      <c r="P17" t="s">
-        <v>38</v>
+      <c r="P17">
+        <v>1</v>
       </c>
       <c r="Q17">
         <v>1</v>

</xml_diff>

<commit_message>
Started work on import/export controller for academic prefs.
</commit_message>
<xml_diff>
--- a/tas/public/template2.xlsx
+++ b/tas/public/template2.xlsx
@@ -16,11 +16,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="49">
   <si>
     <t>Code</t>
   </si>
   <si>
+    <t>CAB201</t>
+  </si>
+  <si>
+    <t>CAB202</t>
+  </si>
+  <si>
+    <t>CAB203</t>
+  </si>
+  <si>
     <t>CAB210</t>
   </si>
   <si>
@@ -42,21 +51,21 @@
     <t>CAB303</t>
   </si>
   <si>
-    <t>CAB202</t>
-  </si>
-  <si>
-    <t>CAB201</t>
-  </si>
-  <si>
-    <t>CAB203</t>
-  </si>
-  <si>
     <t>Standard Load:</t>
   </si>
   <si>
     <t>Name</t>
   </si>
   <si>
+    <t>Programming Principles</t>
+  </si>
+  <si>
+    <t>Micro Proc and Dig Sys</t>
+  </si>
+  <si>
+    <t>Discrete Structures</t>
+  </si>
+  <si>
     <t>People Context &amp; Tech</t>
   </si>
   <si>
@@ -78,15 +87,6 @@
     <t>Networks</t>
   </si>
   <si>
-    <t>Micro Proc and Dig Sys</t>
-  </si>
-  <si>
-    <t>Programming Principles</t>
-  </si>
-  <si>
-    <t>Discrete Structures</t>
-  </si>
-  <si>
     <t>Semester</t>
   </si>
   <si>
@@ -126,15 +126,18 @@
     <t>Load Error</t>
   </si>
   <si>
+    <t xml:space="preserve"> Mantis Tobogan</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t xml:space="preserve"> Kom Poota</t>
   </si>
   <si>
-    <t>CS</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
     <t xml:space="preserve"> Sergine Aldéric </t>
   </si>
   <si>
@@ -150,16 +153,16 @@
     <t xml:space="preserve"> Nia Kerena </t>
   </si>
   <si>
+    <t xml:space="preserve"> Avice Preston </t>
+  </si>
+  <si>
     <t xml:space="preserve"> Hellen Tatianna </t>
   </si>
   <si>
-    <t xml:space="preserve"> Avice Preston </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mantis Tobogan</t>
-  </si>
-  <si>
-    <t>9 Bodies</t>
+    <t>Joel Mehonoshen</t>
+  </si>
+  <si>
+    <t>10 Bodies</t>
   </si>
 </sst>
 </file>
@@ -538,7 +541,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:ZZ19"/>
+  <dimension ref="A1:ZZ20"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="90" zoomScaleNormal="90">
       <selection activeCell="H1" sqref="H1"/>
@@ -569,34 +572,34 @@
         <v>1</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>10</v>
@@ -1290,7 +1293,7 @@
         <v>11</v>
       </c>
       <c r="C2">
-        <f>U6/D19</f>
+        <f>U6/D20</f>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -1299,34 +1302,34 @@
         <v>13</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>22</v>
@@ -2020,7 +2023,7 @@
         <v>23</v>
       </c>
       <c r="H3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I3">
         <v>2</v>
@@ -2035,25 +2038,25 @@
         <v>1</v>
       </c>
       <c r="M3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N3">
         <v>2</v>
       </c>
       <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
         <v>2</v>
       </c>
-      <c r="P3">
-        <v>1</v>
-      </c>
       <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
         <v>2</v>
-      </c>
-      <c r="R3">
-        <v>1</v>
-      </c>
-      <c r="S3">
-        <v>1</v>
       </c>
     </row>
     <row r="4" ht="17.45" customHeight="1" spans="7:19" x14ac:dyDescent="0.25">
@@ -2061,40 +2064,40 @@
         <v>24</v>
       </c>
       <c r="H4">
+        <v>490</v>
+      </c>
+      <c r="I4">
+        <v>610</v>
+      </c>
+      <c r="J4">
+        <v>610</v>
+      </c>
+      <c r="K4">
+        <v>670</v>
+      </c>
+      <c r="L4">
+        <v>680</v>
+      </c>
+      <c r="M4">
         <v>180</v>
       </c>
-      <c r="I4">
+      <c r="N4">
         <v>50</v>
       </c>
-      <c r="J4">
+      <c r="O4">
         <v>400</v>
       </c>
-      <c r="K4">
+      <c r="P4">
         <v>550</v>
       </c>
-      <c r="L4">
+      <c r="Q4">
         <v>500</v>
       </c>
-      <c r="M4">
+      <c r="R4">
         <v>600</v>
       </c>
-      <c r="N4">
+      <c r="S4">
         <v>630</v>
-      </c>
-      <c r="O4">
-        <v>670</v>
-      </c>
-      <c r="P4">
-        <v>490</v>
-      </c>
-      <c r="Q4">
-        <v>610</v>
-      </c>
-      <c r="R4">
-        <v>610</v>
-      </c>
-      <c r="S4">
-        <v>680</v>
       </c>
     </row>
     <row r="5" ht="18" customHeight="1" spans="7:19" x14ac:dyDescent="0.25">
@@ -2105,25 +2108,25 @@
         <v>1</v>
       </c>
       <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>0.6</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
         <v>0.5</v>
       </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
-      <c r="N5">
-        <v>1</v>
-      </c>
       <c r="O5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P5">
         <v>1</v>
@@ -2132,7 +2135,7 @@
         <v>1</v>
       </c>
       <c r="R5">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="S5">
         <v>1</v>
@@ -2149,40 +2152,40 @@
         <v>27</v>
       </c>
       <c r="H6">
+        <v>1.845098</v>
+      </c>
+      <c r="I6">
+        <v>1.9402318</v>
+      </c>
+      <c r="J6">
+        <v>1.164139</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>1.9874109</v>
+      </c>
+      <c r="M6">
         <v>1.4101745</v>
       </c>
-      <c r="I6">
+      <c r="N6">
         <v>0.42693597</v>
       </c>
-      <c r="J6">
+      <c r="O6">
         <v>1.756962</v>
       </c>
-      <c r="K6">
+      <c r="P6">
         <v>1.8952646</v>
       </c>
-      <c r="L6">
+      <c r="Q6">
         <v>1.853872</v>
       </c>
-      <c r="M6">
+      <c r="R6">
         <v>1.9330533</v>
       </c>
-      <c r="N6">
+      <c r="S6">
         <v>1.9542425</v>
-      </c>
-      <c r="O6">
-        <v>NaN</v>
-      </c>
-      <c r="P6">
-        <v>NaN</v>
-      </c>
-      <c r="Q6">
-        <v>NaN</v>
-      </c>
-      <c r="R6">
-        <v>NaN</v>
-      </c>
-      <c r="S6">
-        <v>NaN</v>
       </c>
       <c r="T6" t="s">
         <v>28</v>
@@ -2307,11 +2310,11 @@
       <c r="G9">
         <f>F9-E9</f>
       </c>
-      <c r="H9" t="s">
-        <v>38</v>
-      </c>
-      <c r="I9" t="s">
-        <v>38</v>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
       </c>
       <c r="J9" t="s">
         <v>38</v>
@@ -2331,11 +2334,11 @@
       <c r="O9" t="s">
         <v>38</v>
       </c>
-      <c r="P9">
-        <v>1</v>
-      </c>
-      <c r="Q9">
-        <v>1</v>
+      <c r="P9" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>38</v>
       </c>
       <c r="R9" t="s">
         <v>38</v>
@@ -2363,11 +2366,11 @@
       <c r="G10">
         <f>F10-E10</f>
       </c>
-      <c r="H10" t="s">
-        <v>38</v>
-      </c>
-      <c r="I10" t="s">
-        <v>38</v>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
       </c>
       <c r="J10" t="s">
         <v>38</v>
@@ -2384,8 +2387,8 @@
       <c r="N10" t="s">
         <v>38</v>
       </c>
-      <c r="O10">
-        <v>1</v>
+      <c r="O10" t="s">
+        <v>38</v>
       </c>
       <c r="P10" t="s">
         <v>38</v>
@@ -2393,8 +2396,8 @@
       <c r="Q10" t="s">
         <v>38</v>
       </c>
-      <c r="R10">
-        <v>1</v>
+      <c r="R10" t="s">
+        <v>38</v>
       </c>
       <c r="S10" t="s">
         <v>38</v>
@@ -2425,11 +2428,11 @@
       <c r="I11" t="s">
         <v>38</v>
       </c>
-      <c r="J11" t="s">
-        <v>38</v>
-      </c>
-      <c r="K11" t="s">
-        <v>38</v>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
       </c>
       <c r="L11" t="s">
         <v>38</v>
@@ -2452,8 +2455,8 @@
       <c r="R11" t="s">
         <v>38</v>
       </c>
-      <c r="S11">
-        <v>1</v>
+      <c r="S11" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -2475,11 +2478,11 @@
       <c r="G12">
         <f>F12-E12</f>
       </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
+      <c r="H12" t="s">
+        <v>38</v>
+      </c>
+      <c r="I12" t="s">
+        <v>38</v>
       </c>
       <c r="J12" t="s">
         <v>38</v>
@@ -2487,8 +2490,8 @@
       <c r="K12" t="s">
         <v>38</v>
       </c>
-      <c r="L12" t="s">
-        <v>38</v>
+      <c r="L12">
+        <v>1</v>
       </c>
       <c r="M12" t="s">
         <v>38</v>
@@ -2537,8 +2540,8 @@
       <c r="I13" t="s">
         <v>38</v>
       </c>
-      <c r="J13">
-        <v>1</v>
+      <c r="J13" t="s">
+        <v>38</v>
       </c>
       <c r="K13" t="s">
         <v>38</v>
@@ -2546,11 +2549,11 @@
       <c r="L13" t="s">
         <v>38</v>
       </c>
-      <c r="M13" t="s">
-        <v>38</v>
-      </c>
-      <c r="N13" t="s">
-        <v>38</v>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
       </c>
       <c r="O13" t="s">
         <v>38</v>
@@ -2596,8 +2599,8 @@
       <c r="J14" t="s">
         <v>38</v>
       </c>
-      <c r="K14">
-        <v>1</v>
+      <c r="K14" t="s">
+        <v>38</v>
       </c>
       <c r="L14" t="s">
         <v>38</v>
@@ -2608,8 +2611,8 @@
       <c r="N14" t="s">
         <v>38</v>
       </c>
-      <c r="O14" t="s">
-        <v>38</v>
+      <c r="O14">
+        <v>1</v>
       </c>
       <c r="P14" t="s">
         <v>38</v>
@@ -2658,8 +2661,8 @@
       <c r="L15" t="s">
         <v>38</v>
       </c>
-      <c r="M15">
-        <v>1</v>
+      <c r="M15" t="s">
+        <v>38</v>
       </c>
       <c r="N15" t="s">
         <v>38</v>
@@ -2667,8 +2670,8 @@
       <c r="O15" t="s">
         <v>38</v>
       </c>
-      <c r="P15" t="s">
-        <v>38</v>
+      <c r="P15">
+        <v>1</v>
       </c>
       <c r="Q15" t="s">
         <v>38</v>
@@ -2726,8 +2729,8 @@
       <c r="P16" t="s">
         <v>38</v>
       </c>
-      <c r="Q16" t="s">
-        <v>38</v>
+      <c r="Q16">
+        <v>1</v>
       </c>
       <c r="R16" t="s">
         <v>38</v>
@@ -2779,28 +2782,84 @@
       <c r="O17" t="s">
         <v>38</v>
       </c>
-      <c r="P17">
-        <v>1</v>
-      </c>
-      <c r="Q17">
-        <v>1</v>
-      </c>
-      <c r="R17" t="s">
-        <v>38</v>
+      <c r="P17" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>38</v>
+      </c>
+      <c r="R17">
+        <v>1</v>
       </c>
       <c r="S17" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>47</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18">
+        <v>21</v>
+      </c>
+      <c r="E18">
+        <f>D18*$C$2</f>
+      </c>
+      <c r="F18">
+        <f>SUMPRODUCT(H$6:T$6,H9:T9)</f>
+      </c>
+      <c r="G18">
+        <f>F18-E18</f>
+      </c>
+      <c r="H18" t="s">
+        <v>38</v>
+      </c>
+      <c r="I18" t="s">
+        <v>38</v>
+      </c>
+      <c r="J18" t="s">
+        <v>38</v>
+      </c>
+      <c r="K18" t="s">
+        <v>38</v>
+      </c>
+      <c r="L18" t="s">
+        <v>38</v>
+      </c>
+      <c r="M18" t="s">
+        <v>38</v>
+      </c>
+      <c r="N18" t="s">
+        <v>38</v>
+      </c>
+      <c r="O18" t="s">
+        <v>38</v>
+      </c>
+      <c r="P18" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>38</v>
+      </c>
+      <c r="R18" t="s">
+        <v>38</v>
+      </c>
+      <c r="S18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" t="s">
         <v>28</v>
       </c>
-      <c r="D19">
-        <f>SUM(D9:D18)</f>
+      <c r="D20">
+        <f>SUM(D9:D19)</f>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added sort + filter buttons for Allocations page,  but doesn't work yet
</commit_message>
<xml_diff>
--- a/tas/public/template2.xlsx
+++ b/tas/public/template2.xlsx
@@ -19,9 +19,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6574" uniqueCount="190">
   <si>
     <t>Code</t>
-  </si>
-  <si>
-    <t>CAB000</t>
   </si>
   <si>
     <t>CAB201</t>
@@ -61,9 +58,6 @@
   </si>
   <si>
     <t>CAB340</t>
-  </si>
-  <si>
-    <t>CAB401</t>
   </si>
   <si>
     <t>CAB402</t>
@@ -228,13 +222,16 @@
     <t>IGB400</t>
   </si>
   <si>
+    <t>CAB000</t>
+  </si>
+  <si>
+    <t>CAB401</t>
+  </si>
+  <si>
     <t>Standard Load:</t>
   </si>
   <si>
     <t>Name</t>
-  </si>
-  <si>
-    <t>Test</t>
   </si>
   <si>
     <t>Programming Principles</t>
@@ -274,9 +271,6 @@
   </si>
   <si>
     <t>Cryptography</t>
-  </si>
-  <si>
-    <t>High Performance and Parallel Computing</t>
   </si>
   <si>
     <t>Programming Paradigms</t>
@@ -418,6 +412,12 @@
   </si>
   <si>
     <t>Game Studio 3</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>High Performance and Parallel Computing</t>
   </si>
   <si>
     <t>Semester</t>
@@ -998,7 +998,7 @@
         <v>2</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>3</v>
@@ -1067,22 +1067,22 @@
         <v>24</v>
       </c>
       <c r="AG1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AH1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="AM1" s="1" t="s">
         <v>28</v>
@@ -1103,28 +1103,28 @@
         <v>33</v>
       </c>
       <c r="AS1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AT1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AV1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="AY1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="BA1" s="1" t="s">
         <v>38</v>
@@ -1172,16 +1172,16 @@
         <v>52</v>
       </c>
       <c r="BP1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BQ1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="BQ1" s="1" t="s">
+      <c r="BR1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="BS1" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="BR1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="BS1" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="BT1" s="1" t="s">
         <v>55</v>
@@ -1229,247 +1229,247 @@
         <v>69</v>
       </c>
       <c r="CI1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="CJ1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="CK1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="CL1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="CM1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="CN1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="CO1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="CP1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="CQ1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="CR1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="CS1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="CT1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="CU1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="CV1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="CW1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="CX1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="CY1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="CZ1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="DA1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="DB1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="DC1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="DD1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="DE1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="DF1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="DG1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="DH1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="DI1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="DJ1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="DK1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="DL1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="CJ1" s="1" t="s">
+      <c r="DM1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="CK1" s="1" t="s">
+      <c r="DN1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="CL1" s="1" t="s">
+      <c r="DO1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="DP1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="DQ1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="DR1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="DS1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="DT1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="DU1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="DV1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="DW1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="DX1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="DY1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="DZ1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="EA1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="EB1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="EC1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="ED1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="EE1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="EF1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="EG1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="EH1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="EI1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="EJ1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="EK1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="EL1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="EM1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="EN1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="EO1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="EP1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="EQ1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="ER1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="ES1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="ET1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="CM1" s="1" t="s">
+      <c r="EU1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="CN1" s="1" t="s">
+      <c r="EV1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="CO1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="CP1" s="1" t="s">
+      <c r="EW1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="EX1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="CQ1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="CR1" s="1" t="s">
+      <c r="EY1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="EZ1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="FA1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="CS1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="CT1" s="1" t="s">
+      <c r="FB1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="CU1" s="1" t="s">
+      <c r="FC1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="CV1" s="1" t="s">
+      <c r="FD1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="CW1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="CX1" s="1" t="s">
+      <c r="FE1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="FF1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="CY1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="CZ1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="DA1" s="1" t="s">
+      <c r="FG1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="FH1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="FI1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="DB1" s="1" t="s">
+      <c r="FJ1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="DC1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="DD1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="DE1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="DF1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="DG1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="DH1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="DI1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="DJ1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="DK1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="DL1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="DM1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="DN1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="DO1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="DP1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="DQ1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="DR1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="DS1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="DT1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="DU1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="DV1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="DW1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="DX1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="DY1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="DZ1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="EA1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="EB1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="EC1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="ED1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="EE1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="EF1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="EG1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="EH1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="EI1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="EJ1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="EK1" s="1" t="s">
+      <c r="FK1" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="EL1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="EM1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="EN1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="EO1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="EP1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="EQ1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="ER1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="ES1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="ET1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="EU1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="EV1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="EW1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="EX1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="EY1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="EZ1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="FA1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="FB1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="FC1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="FD1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="FE1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="FF1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="FG1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="FH1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="FI1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="FJ1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="FK1" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="FL1" s="1"/>
       <c r="FM1" s="1"/>
@@ -2024,7 +2024,7 @@
         <v>73</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>74</v>
@@ -2093,82 +2093,82 @@
         <v>95</v>
       </c>
       <c r="AG2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AH2" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="AH2" s="1" t="s">
+      <c r="AI2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="AI2" s="1" t="s">
+      <c r="AK2" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="AJ2" s="1" t="s">
+      <c r="AL2" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="AK2" s="1" t="s">
+      <c r="AM2" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="AL2" s="1" t="s">
+      <c r="AN2" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="AM2" s="1" t="s">
+      <c r="AO2" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="AN2" s="1" t="s">
+      <c r="AP2" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AO2" s="1" t="s">
+      <c r="AQ2" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="AP2" s="1" t="s">
+      <c r="AR2" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="AQ2" s="1" t="s">
+      <c r="AS2" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="AR2" s="1" t="s">
+      <c r="AT2" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="AS2" s="1" t="s">
+      <c r="AU2" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="AT2" s="1" t="s">
+      <c r="AV2" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="AU2" s="1" t="s">
+      <c r="AW2" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="AV2" s="1" t="s">
+      <c r="AX2" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="AW2" s="1" t="s">
+      <c r="AY2" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="AX2" s="1" t="s">
+      <c r="AZ2" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="AY2" s="1" t="s">
+      <c r="BA2" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="AZ2" s="1" t="s">
+      <c r="BB2" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="BA2" s="1" t="s">
+      <c r="BC2" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="BB2" s="1" t="s">
+      <c r="BD2" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="BC2" s="1" t="s">
+      <c r="BE2" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="BD2" s="1" t="s">
+      <c r="BF2" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="BE2" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="BF2" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="BG2" s="1" t="s">
         <v>109</v>
@@ -2198,16 +2198,16 @@
         <v>117</v>
       </c>
       <c r="BP2" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="BQ2" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="BR2" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="BS2" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="BQ2" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="BR2" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="BS2" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="BT2" s="1" t="s">
         <v>119</v>
@@ -2255,247 +2255,247 @@
         <v>133</v>
       </c>
       <c r="CI2" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="CJ2" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="CK2" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="CL2" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="CM2" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="CN2" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="CO2" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="CP2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="CQ2" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="CQ2" s="1" t="s">
+      <c r="CR2" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="CR2" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="CS2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="CT2" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="CT2" s="1" t="s">
+      <c r="CU2" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="CU2" s="1" t="s">
-        <v>108</v>
-      </c>
       <c r="CV2" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="CW2" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="CX2" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="CY2" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="CZ2" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="DA2" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="DB2" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="DC2" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="DD2" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="DE2" s="1" t="s">
-        <v>73</v>
+        <v>132</v>
       </c>
       <c r="DF2" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="DG2" s="1" t="s">
         <v>72</v>
       </c>
       <c r="DH2" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="DI2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="DJ2" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="DI2" s="1" t="s">
+      <c r="DK2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="DL2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="DM2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="DN2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="DO2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="DP2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="DQ2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="DR2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="DS2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="DT2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="DU2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="DV2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="DW2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="DX2" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="DY2" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="DZ2" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="EA2" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="EB2" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="EC2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="ED2" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="EE2" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="EF2" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="EG2" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="EH2" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="EI2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="EJ2" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="EK2" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="EL2" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="EM2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="EN2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="EO2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="DJ2" s="1" t="s">
+      <c r="EP2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="DK2" s="1" t="s">
+      <c r="EQ2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="DL2" s="1" t="s">
+      <c r="ER2" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="DM2" s="1" t="s">
+      <c r="ES2" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="DN2" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="DO2" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="DP2" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="DQ2" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="DR2" s="1" t="s">
+      <c r="ET2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="EU2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="EV2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="EW2" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="DS2" s="1" t="s">
+      <c r="EX2" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="DT2" s="1" t="s">
+      <c r="EY2" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="DU2" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="DV2" s="1" t="s">
+      <c r="EZ2" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="DW2" s="1" t="s">
+      <c r="FA2" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="DX2" s="1" t="s">
+      <c r="FB2" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="DY2" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="DZ2" s="1" t="s">
+      <c r="FC2" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="EA2" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="EB2" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="EC2" s="1" t="s">
+      <c r="FD2" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="FE2" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="ED2" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="EE2" s="1" t="s">
+      <c r="FF2" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="FG2" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="EF2" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="EG2" s="1" t="s">
+      <c r="FH2" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="EH2" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="EI2" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="EJ2" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="EK2" s="1" t="s">
+      <c r="FI2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="FJ2" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="FK2" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="EL2" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="EM2" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="EN2" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="EO2" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="EP2" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="EQ2" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="ER2" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="ES2" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="ET2" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="EU2" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="EV2" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="EW2" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="EX2" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="EY2" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="EZ2" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="FA2" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="FB2" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="FC2" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="FD2" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="FE2" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="FF2" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="FG2" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="FH2" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="FI2" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="FJ2" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="FK2" s="1" t="s">
-        <v>132</v>
       </c>
       <c r="FL2" s="1"/>
       <c r="FM2" s="1"/>
@@ -3038,49 +3038,49 @@
         <v>134</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
         <v>2</v>
       </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
       <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
         <v>2</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
       </c>
       <c r="M3">
         <v>2</v>
       </c>
       <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
         <v>2</v>
       </c>
-      <c r="O3">
-        <v>1</v>
-      </c>
       <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
         <v>2</v>
       </c>
-      <c r="Q3">
-        <v>1</v>
-      </c>
-      <c r="R3">
-        <v>1</v>
-      </c>
       <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
         <v>2</v>
-      </c>
-      <c r="T3">
-        <v>1</v>
       </c>
       <c r="U3">
         <v>2</v>
       </c>
       <c r="V3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W3">
         <v>2</v>
@@ -3089,10 +3089,10 @@
         <v>1</v>
       </c>
       <c r="Y3">
+        <v>1</v>
+      </c>
+      <c r="Z3">
         <v>2</v>
-      </c>
-      <c r="Z3">
-        <v>1</v>
       </c>
       <c r="AA3">
         <v>1</v>
@@ -3107,10 +3107,10 @@
         <v>2</v>
       </c>
       <c r="AE3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AG3">
         <v>2</v>
@@ -3191,19 +3191,19 @@
         <v>1</v>
       </c>
       <c r="BG3">
+        <v>1</v>
+      </c>
+      <c r="BH3">
         <v>2</v>
       </c>
-      <c r="BH3">
-        <v>1</v>
-      </c>
       <c r="BI3">
         <v>1</v>
       </c>
       <c r="BJ3">
+        <v>1</v>
+      </c>
+      <c r="BK3">
         <v>2</v>
-      </c>
-      <c r="BK3">
-        <v>1</v>
       </c>
       <c r="BL3">
         <v>1</v>
@@ -3212,10 +3212,10 @@
         <v>2</v>
       </c>
       <c r="BN3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BO3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BP3">
         <v>2</v>
@@ -3227,28 +3227,28 @@
         <v>2</v>
       </c>
       <c r="BS3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BT3">
+        <v>1</v>
+      </c>
+      <c r="BU3">
+        <v>1</v>
+      </c>
+      <c r="BV3">
+        <v>1</v>
+      </c>
+      <c r="BW3">
         <v>2</v>
       </c>
-      <c r="BU3">
+      <c r="BX3">
         <v>2</v>
-      </c>
-      <c r="BV3">
-        <v>1</v>
-      </c>
-      <c r="BW3">
-        <v>1</v>
-      </c>
-      <c r="BX3">
-        <v>1</v>
       </c>
       <c r="BY3">
         <v>2</v>
       </c>
       <c r="BZ3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="CA3">
         <v>2</v>
@@ -3260,10 +3260,10 @@
         <v>2</v>
       </c>
       <c r="CD3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="CE3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="CF3">
         <v>2</v>
@@ -3350,22 +3350,22 @@
         <v>1</v>
       </c>
       <c r="DH3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="DI3">
         <v>1</v>
       </c>
       <c r="DJ3">
+        <v>1</v>
+      </c>
+      <c r="DK3">
         <v>2</v>
       </c>
-      <c r="DK3">
-        <v>1</v>
-      </c>
       <c r="DL3">
         <v>1</v>
       </c>
       <c r="DM3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="DN3">
         <v>1</v>
@@ -3523,118 +3523,118 @@
         <v>135</v>
       </c>
       <c r="H4">
-        <v>100</v>
+        <v>610</v>
       </c>
       <c r="I4">
         <v>610</v>
       </c>
       <c r="J4">
-        <v>610</v>
+        <v>670</v>
       </c>
       <c r="K4">
-        <v>670</v>
+        <v>680</v>
       </c>
       <c r="L4">
-        <v>680</v>
+        <v>180</v>
       </c>
       <c r="M4">
-        <v>180</v>
+        <v>50</v>
       </c>
       <c r="N4">
-        <v>50</v>
+        <v>400</v>
       </c>
       <c r="O4">
-        <v>400</v>
+        <v>550</v>
       </c>
       <c r="P4">
-        <v>550</v>
+        <v>500</v>
       </c>
       <c r="Q4">
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="R4">
-        <v>600</v>
+        <v>630</v>
       </c>
       <c r="S4">
-        <v>630</v>
+        <v>40</v>
       </c>
       <c r="T4">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="U4">
-        <v>60</v>
+        <v>140</v>
       </c>
       <c r="V4">
         <v>140</v>
       </c>
       <c r="W4">
-        <v>150</v>
+        <v>350</v>
       </c>
       <c r="X4">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="Y4">
-        <v>350</v>
+        <v>35</v>
       </c>
       <c r="Z4">
-        <v>40</v>
+        <v>180</v>
       </c>
       <c r="AA4">
-        <v>35</v>
+        <v>130</v>
       </c>
       <c r="AB4">
-        <v>180</v>
+        <v>85</v>
       </c>
       <c r="AC4">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="AD4">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="AE4">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="AF4">
+        <v>800</v>
+      </c>
+      <c r="AG4">
+        <v>275</v>
+      </c>
+      <c r="AH4">
+        <v>720</v>
+      </c>
+      <c r="AI4">
+        <v>710</v>
+      </c>
+      <c r="AJ4">
+        <v>450</v>
+      </c>
+      <c r="AK4">
+        <v>170</v>
+      </c>
+      <c r="AL4">
+        <v>81</v>
+      </c>
+      <c r="AM4">
+        <v>81</v>
+      </c>
+      <c r="AN4">
         <v>80</v>
       </c>
-      <c r="AG4">
-        <v>120</v>
-      </c>
-      <c r="AH4">
-        <v>800</v>
-      </c>
-      <c r="AI4">
-        <v>275</v>
-      </c>
-      <c r="AJ4">
-        <v>720</v>
-      </c>
-      <c r="AK4">
-        <v>710</v>
-      </c>
-      <c r="AL4">
-        <v>450</v>
-      </c>
-      <c r="AM4">
-        <v>170</v>
-      </c>
-      <c r="AN4">
-        <v>81</v>
-      </c>
       <c r="AO4">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AP4">
-        <v>80</v>
+        <v>53</v>
       </c>
       <c r="AQ4">
-        <v>80</v>
+        <v>53</v>
       </c>
       <c r="AR4">
-        <v>53</v>
+        <v>108</v>
       </c>
       <c r="AS4">
-        <v>53</v>
+        <v>108</v>
       </c>
       <c r="AT4">
         <v>108</v>
@@ -3646,7 +3646,7 @@
         <v>108</v>
       </c>
       <c r="AW4">
-        <v>108</v>
+        <v>54</v>
       </c>
       <c r="AX4">
         <v>108</v>
@@ -3655,10 +3655,10 @@
         <v>54</v>
       </c>
       <c r="AZ4">
-        <v>108</v>
+        <v>70</v>
       </c>
       <c r="BA4">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="BB4">
         <v>70</v>
@@ -3673,37 +3673,37 @@
         <v>70</v>
       </c>
       <c r="BF4">
+        <v>88</v>
+      </c>
+      <c r="BG4">
+        <v>135</v>
+      </c>
+      <c r="BH4">
         <v>70</v>
       </c>
-      <c r="BG4">
+      <c r="BI4">
+        <v>140</v>
+      </c>
+      <c r="BJ4">
+        <v>74</v>
+      </c>
+      <c r="BK4">
+        <v>136</v>
+      </c>
+      <c r="BL4">
         <v>70</v>
       </c>
-      <c r="BH4">
-        <v>88</v>
-      </c>
-      <c r="BI4">
-        <v>135</v>
-      </c>
-      <c r="BJ4">
-        <v>70</v>
-      </c>
-      <c r="BK4">
-        <v>140</v>
-      </c>
-      <c r="BL4">
-        <v>74</v>
-      </c>
       <c r="BM4">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="BN4">
         <v>70</v>
       </c>
       <c r="BO4">
-        <v>139</v>
+        <v>40</v>
       </c>
       <c r="BP4">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="BQ4">
         <v>40</v>
@@ -3712,52 +3712,52 @@
         <v>40</v>
       </c>
       <c r="BS4">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="BT4">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="BU4">
-        <v>200</v>
+        <v>280</v>
       </c>
       <c r="BV4">
+        <v>158</v>
+      </c>
+      <c r="BW4">
+        <v>69</v>
+      </c>
+      <c r="BX4">
+        <v>121</v>
+      </c>
+      <c r="BY4">
+        <v>70</v>
+      </c>
+      <c r="BZ4">
+        <v>74</v>
+      </c>
+      <c r="CA4">
+        <v>74</v>
+      </c>
+      <c r="CB4">
+        <v>50</v>
+      </c>
+      <c r="CC4">
+        <v>59</v>
+      </c>
+      <c r="CD4">
+        <v>36</v>
+      </c>
+      <c r="CE4">
+        <v>36</v>
+      </c>
+      <c r="CF4">
+        <v>77</v>
+      </c>
+      <c r="CG4">
         <v>100</v>
       </c>
-      <c r="BW4">
-        <v>280</v>
-      </c>
-      <c r="BX4">
-        <v>158</v>
-      </c>
-      <c r="BY4">
-        <v>69</v>
-      </c>
-      <c r="BZ4">
-        <v>121</v>
-      </c>
-      <c r="CA4">
-        <v>70</v>
-      </c>
-      <c r="CB4">
-        <v>74</v>
-      </c>
-      <c r="CC4">
-        <v>74</v>
-      </c>
-      <c r="CD4">
-        <v>50</v>
-      </c>
-      <c r="CE4">
-        <v>59</v>
-      </c>
-      <c r="CF4">
-        <v>36</v>
-      </c>
-      <c r="CG4">
-        <v>36</v>
-      </c>
       <c r="CH4">
-        <v>77</v>
+        <v>150</v>
       </c>
       <c r="CI4">
         <v>550</v>
@@ -3826,31 +3826,31 @@
         <v>77</v>
       </c>
       <c r="DE4">
-        <v>490</v>
+        <v>100</v>
       </c>
       <c r="DF4">
         <v>490</v>
       </c>
       <c r="DG4">
-        <v>100</v>
+        <v>490</v>
       </c>
       <c r="DH4">
+        <v>150</v>
+      </c>
+      <c r="DI4">
         <v>610</v>
       </c>
-      <c r="DI4">
+      <c r="DJ4">
         <v>680</v>
       </c>
-      <c r="DJ4">
+      <c r="DK4">
         <v>50</v>
       </c>
-      <c r="DK4">
+      <c r="DL4">
         <v>500</v>
       </c>
-      <c r="DL4">
+      <c r="DM4">
         <v>40</v>
-      </c>
-      <c r="DM4">
-        <v>150</v>
       </c>
       <c r="DN4">
         <v>140</v>
@@ -4011,115 +4011,115 @@
         <v>1</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="J5">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>0.5</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <v>1</v>
+      </c>
+      <c r="T5">
+        <v>1</v>
+      </c>
+      <c r="U5">
+        <v>1</v>
+      </c>
+      <c r="V5">
+        <v>1</v>
+      </c>
+      <c r="W5">
+        <v>1</v>
+      </c>
+      <c r="X5">
+        <v>1</v>
+      </c>
+      <c r="Y5">
+        <v>1</v>
+      </c>
+      <c r="Z5">
+        <v>1</v>
+      </c>
+      <c r="AA5">
+        <v>1</v>
+      </c>
+      <c r="AB5">
+        <v>1</v>
+      </c>
+      <c r="AC5">
+        <v>1</v>
+      </c>
+      <c r="AD5">
+        <v>1</v>
+      </c>
+      <c r="AE5">
         <v>0</v>
       </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
-      <c r="N5">
+      <c r="AF5">
+        <v>1</v>
+      </c>
+      <c r="AG5">
+        <v>1</v>
+      </c>
+      <c r="AH5">
+        <v>1</v>
+      </c>
+      <c r="AI5">
+        <v>1</v>
+      </c>
+      <c r="AJ5">
+        <v>1</v>
+      </c>
+      <c r="AK5">
+        <v>1</v>
+      </c>
+      <c r="AL5">
+        <v>1</v>
+      </c>
+      <c r="AM5">
+        <v>1.2</v>
+      </c>
+      <c r="AN5">
+        <v>1</v>
+      </c>
+      <c r="AO5">
+        <v>1</v>
+      </c>
+      <c r="AP5">
+        <v>1</v>
+      </c>
+      <c r="AQ5">
+        <v>1.2</v>
+      </c>
+      <c r="AR5">
+        <v>0.7</v>
+      </c>
+      <c r="AS5">
         <v>0.5</v>
-      </c>
-      <c r="O5">
-        <v>1</v>
-      </c>
-      <c r="P5">
-        <v>1</v>
-      </c>
-      <c r="Q5">
-        <v>1</v>
-      </c>
-      <c r="R5">
-        <v>1</v>
-      </c>
-      <c r="S5">
-        <v>1</v>
-      </c>
-      <c r="T5">
-        <v>1</v>
-      </c>
-      <c r="U5">
-        <v>1</v>
-      </c>
-      <c r="V5">
-        <v>1</v>
-      </c>
-      <c r="W5">
-        <v>1</v>
-      </c>
-      <c r="X5">
-        <v>1</v>
-      </c>
-      <c r="Y5">
-        <v>1</v>
-      </c>
-      <c r="Z5">
-        <v>1</v>
-      </c>
-      <c r="AA5">
-        <v>1</v>
-      </c>
-      <c r="AB5">
-        <v>1</v>
-      </c>
-      <c r="AC5">
-        <v>1</v>
-      </c>
-      <c r="AD5">
-        <v>1</v>
-      </c>
-      <c r="AE5">
-        <v>1</v>
-      </c>
-      <c r="AF5">
-        <v>1</v>
-      </c>
-      <c r="AG5">
-        <v>0</v>
-      </c>
-      <c r="AH5">
-        <v>1</v>
-      </c>
-      <c r="AI5">
-        <v>1</v>
-      </c>
-      <c r="AJ5">
-        <v>1</v>
-      </c>
-      <c r="AK5">
-        <v>1</v>
-      </c>
-      <c r="AL5">
-        <v>1</v>
-      </c>
-      <c r="AM5">
-        <v>1</v>
-      </c>
-      <c r="AN5">
-        <v>1</v>
-      </c>
-      <c r="AO5">
-        <v>1.2</v>
-      </c>
-      <c r="AP5">
-        <v>1</v>
-      </c>
-      <c r="AQ5">
-        <v>1</v>
-      </c>
-      <c r="AR5">
-        <v>1</v>
-      </c>
-      <c r="AS5">
-        <v>1.2</v>
       </c>
       <c r="AT5">
         <v>0.7</v>
@@ -4140,7 +4140,7 @@
         <v>0.5</v>
       </c>
       <c r="AZ5">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="BA5">
         <v>0.5</v>
@@ -4152,40 +4152,40 @@
         <v>0.5</v>
       </c>
       <c r="BD5">
+        <v>1</v>
+      </c>
+      <c r="BE5">
+        <v>1</v>
+      </c>
+      <c r="BF5">
+        <v>1</v>
+      </c>
+      <c r="BG5">
+        <v>1</v>
+      </c>
+      <c r="BH5">
+        <v>1</v>
+      </c>
+      <c r="BI5">
+        <v>1</v>
+      </c>
+      <c r="BJ5">
+        <v>1</v>
+      </c>
+      <c r="BK5">
+        <v>1</v>
+      </c>
+      <c r="BL5">
+        <v>1</v>
+      </c>
+      <c r="BM5">
         <v>0.5</v>
       </c>
-      <c r="BE5">
-        <v>0.5</v>
-      </c>
-      <c r="BF5">
-        <v>1</v>
-      </c>
-      <c r="BG5">
-        <v>1</v>
-      </c>
-      <c r="BH5">
-        <v>1</v>
-      </c>
-      <c r="BI5">
-        <v>1</v>
-      </c>
-      <c r="BJ5">
-        <v>1</v>
-      </c>
-      <c r="BK5">
-        <v>1</v>
-      </c>
-      <c r="BL5">
-        <v>1</v>
-      </c>
-      <c r="BM5">
-        <v>1</v>
-      </c>
       <c r="BN5">
         <v>1</v>
       </c>
       <c r="BO5">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="BP5">
         <v>1</v>
@@ -4311,25 +4311,25 @@
         <v>1</v>
       </c>
       <c r="DE5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="DF5">
         <v>1</v>
       </c>
       <c r="DG5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="DH5">
+        <v>1</v>
+      </c>
+      <c r="DI5">
         <v>0.6</v>
       </c>
-      <c r="DI5">
-        <v>1</v>
-      </c>
       <c r="DJ5">
+        <v>1</v>
+      </c>
+      <c r="DK5">
         <v>0.5</v>
-      </c>
-      <c r="DK5">
-        <v>1</v>
       </c>
       <c r="DL5">
         <v>1</v>
@@ -4499,118 +4499,118 @@
         <v>138</v>
       </c>
       <c r="H6">
-        <v>1.154902</v>
+        <v>1.9402318</v>
       </c>
       <c r="I6">
-        <v>1.9402318</v>
+        <v>1.164139</v>
       </c>
       <c r="J6">
-        <v>1.164139</v>
+        <v>0</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>1.9874109</v>
       </c>
       <c r="L6">
-        <v>1.9874109</v>
+        <v>1.4101745</v>
       </c>
       <c r="M6">
-        <v>1.4101745</v>
+        <v>0.42693597</v>
       </c>
       <c r="N6">
-        <v>0.42693597</v>
+        <v>1.756962</v>
       </c>
       <c r="O6">
-        <v>1.756962</v>
+        <v>1.8952646</v>
       </c>
       <c r="P6">
-        <v>1.8952646</v>
+        <v>1.853872</v>
       </c>
       <c r="Q6">
-        <v>1.853872</v>
+        <v>1.9330533</v>
       </c>
       <c r="R6">
-        <v>1.9330533</v>
+        <v>1.9542425</v>
       </c>
       <c r="S6">
-        <v>1.9542425</v>
+        <v>0.8</v>
       </c>
       <c r="T6">
-        <v>0.8</v>
+        <v>0.9330532</v>
       </c>
       <c r="U6">
-        <v>0.9330532</v>
+        <v>1.30103</v>
       </c>
       <c r="V6">
         <v>1.30103</v>
       </c>
       <c r="W6">
-        <v>1.3309932</v>
+        <v>1.69897</v>
       </c>
       <c r="X6">
-        <v>1.30103</v>
+        <v>0.8</v>
       </c>
       <c r="Y6">
-        <v>1.69897</v>
+        <v>0.8</v>
       </c>
       <c r="Z6">
-        <v>0.8</v>
+        <v>1.4101745</v>
       </c>
       <c r="AA6">
-        <v>0.8</v>
+        <v>1.2688453</v>
       </c>
       <c r="AB6">
-        <v>1.4101745</v>
+        <v>1.0843209</v>
       </c>
       <c r="AC6">
-        <v>1.2688453</v>
+        <v>1.154902</v>
       </c>
       <c r="AD6">
-        <v>1.0843209</v>
+        <v>1.057992</v>
       </c>
       <c r="AE6">
-        <v>1.154902</v>
+        <v>0</v>
       </c>
       <c r="AF6">
+        <v>2.057992</v>
+      </c>
+      <c r="AG6">
+        <v>1.5942347</v>
+      </c>
+      <c r="AH6">
+        <v>2.0122344</v>
+      </c>
+      <c r="AI6">
+        <v>2.0061603</v>
+      </c>
+      <c r="AJ6">
+        <v>1.8081145</v>
+      </c>
+      <c r="AK6">
+        <v>1.3853508</v>
+      </c>
+      <c r="AL6">
+        <v>1.063387</v>
+      </c>
+      <c r="AM6">
+        <v>1.2760644</v>
+      </c>
+      <c r="AN6">
         <v>1.057992</v>
       </c>
-      <c r="AG6">
-        <v>0</v>
-      </c>
-      <c r="AH6">
-        <v>2.057992</v>
-      </c>
-      <c r="AI6">
-        <v>1.5942347</v>
-      </c>
-      <c r="AJ6">
-        <v>2.0122344</v>
-      </c>
-      <c r="AK6">
-        <v>2.0061603</v>
-      </c>
-      <c r="AL6">
-        <v>1.8081145</v>
-      </c>
-      <c r="AM6">
-        <v>1.3853508</v>
-      </c>
-      <c r="AN6">
-        <v>1.063387</v>
-      </c>
       <c r="AO6">
-        <v>1.2760644</v>
+        <v>1.057992</v>
       </c>
       <c r="AP6">
-        <v>1.057992</v>
+        <v>0.8791778</v>
       </c>
       <c r="AQ6">
-        <v>1.057992</v>
+        <v>1.0550134</v>
       </c>
       <c r="AR6">
-        <v>0.8791778</v>
+        <v>0.831828</v>
       </c>
       <c r="AS6">
-        <v>1.0550134</v>
+        <v>0.5941629</v>
       </c>
       <c r="AT6">
         <v>0.831828</v>
@@ -4622,7 +4622,7 @@
         <v>0.831828</v>
       </c>
       <c r="AW6">
-        <v>0.5941629</v>
+        <v>0.44364786</v>
       </c>
       <c r="AX6">
         <v>0.831828</v>
@@ -4631,10 +4631,10 @@
         <v>0.44364786</v>
       </c>
       <c r="AZ6">
-        <v>0.831828</v>
+        <v>0.5</v>
       </c>
       <c r="BA6">
-        <v>0.44364786</v>
+        <v>0.5</v>
       </c>
       <c r="BB6">
         <v>0.5</v>
@@ -4643,43 +4643,43 @@
         <v>0.5</v>
       </c>
       <c r="BD6">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="BE6">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="BF6">
-        <v>1</v>
+        <v>1.0993847</v>
       </c>
       <c r="BG6">
-        <v>1</v>
+        <v>1.2852358</v>
       </c>
       <c r="BH6">
-        <v>1.0993847</v>
+        <v>1</v>
       </c>
       <c r="BI6">
-        <v>1.2852358</v>
+        <v>1.30103</v>
       </c>
       <c r="BJ6">
-        <v>1</v>
+        <v>1.0241337</v>
       </c>
       <c r="BK6">
-        <v>1.30103</v>
+        <v>1.2884408</v>
       </c>
       <c r="BL6">
-        <v>1.0241337</v>
+        <v>1</v>
       </c>
       <c r="BM6">
-        <v>1.2884408</v>
+        <v>0.6489584</v>
       </c>
       <c r="BN6">
         <v>1</v>
       </c>
       <c r="BO6">
-        <v>0.6489584</v>
+        <v>0.8</v>
       </c>
       <c r="BP6">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="BQ6">
         <v>0.8</v>
@@ -4688,52 +4688,52 @@
         <v>0.8</v>
       </c>
       <c r="BS6">
+        <v>1.4559319</v>
+      </c>
+      <c r="BT6">
+        <v>1.154902</v>
+      </c>
+      <c r="BU6">
+        <v>1.60206</v>
+      </c>
+      <c r="BV6">
+        <v>1.353559</v>
+      </c>
+      <c r="BW6">
+        <v>0.99375105</v>
+      </c>
+      <c r="BX6">
+        <v>1.2376873</v>
+      </c>
+      <c r="BY6">
+        <v>1</v>
+      </c>
+      <c r="BZ6">
+        <v>1.0241337</v>
+      </c>
+      <c r="CA6">
+        <v>1.0241337</v>
+      </c>
+      <c r="CB6">
+        <v>0.85387194</v>
+      </c>
+      <c r="CC6">
+        <v>0.92575395</v>
+      </c>
+      <c r="CD6">
         <v>0.8</v>
       </c>
-      <c r="BT6">
+      <c r="CE6">
         <v>0.8</v>
       </c>
-      <c r="BU6">
-        <v>1.4559319</v>
-      </c>
-      <c r="BV6">
-        <v>1.154902</v>
-      </c>
-      <c r="BW6">
-        <v>1.60206</v>
-      </c>
-      <c r="BX6">
-        <v>1.353559</v>
-      </c>
-      <c r="BY6">
-        <v>0.99375105</v>
-      </c>
-      <c r="BZ6">
-        <v>1.2376873</v>
-      </c>
-      <c r="CA6">
-        <v>1</v>
-      </c>
-      <c r="CB6">
-        <v>1.0241337</v>
-      </c>
-      <c r="CC6">
-        <v>1.0241337</v>
-      </c>
-      <c r="CD6">
-        <v>0.85387194</v>
-      </c>
-      <c r="CE6">
-        <v>0.92575395</v>
-      </c>
       <c r="CF6">
-        <v>0.8</v>
+        <v>1.0413927</v>
       </c>
       <c r="CG6">
-        <v>0.8</v>
+        <v>NaN</v>
       </c>
       <c r="CH6">
-        <v>1.0413927</v>
+        <v>NaN</v>
       </c>
       <c r="CI6">
         <v>1.8952646</v>
@@ -4808,25 +4808,25 @@
         <v>NaN</v>
       </c>
       <c r="DG6">
-        <v>2.309804</v>
+        <v>NaN</v>
       </c>
       <c r="DH6">
+        <v>NaN</v>
+      </c>
+      <c r="DI6">
         <v>1.164139</v>
       </c>
-      <c r="DI6">
+      <c r="DJ6">
         <v>1.9874109</v>
       </c>
-      <c r="DJ6">
+      <c r="DK6">
         <v>0.42693597</v>
       </c>
-      <c r="DK6">
+      <c r="DL6">
         <v>1.853872</v>
       </c>
-      <c r="DL6">
+      <c r="DM6">
         <v>0.8</v>
-      </c>
-      <c r="DM6">
-        <v>1.3309932</v>
       </c>
       <c r="DN6">
         <v>1.30103</v>
@@ -5989,14 +5989,17 @@
       <c r="G9">
         <f>F9-E9</f>
       </c>
+      <c r="H9">
+        <v>0.1</v>
+      </c>
       <c r="I9">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="J9">
         <v>1</v>
       </c>
-      <c r="K9">
-        <v>1</v>
+      <c r="K9" t="s">
+        <v>149</v>
       </c>
       <c r="L9" t="s">
         <v>149</v>
@@ -6016,12 +6019,12 @@
       <c r="Q9" t="s">
         <v>149</v>
       </c>
-      <c r="R9" t="s">
-        <v>149</v>
-      </c>
-      <c r="S9">
+      <c r="R9">
         <v>0.2</v>
       </c>
+      <c r="S9" t="s">
+        <v>149</v>
+      </c>
       <c r="T9" t="s">
         <v>149</v>
       </c>
@@ -6215,9 +6218,6 @@
         <v>149</v>
       </c>
       <c r="CF9" t="s">
-        <v>149</v>
-      </c>
-      <c r="CG9" t="s">
         <v>149</v>
       </c>
       <c r="CH9" t="s">
@@ -6289,17 +6289,17 @@
       <c r="DD9" t="s">
         <v>149</v>
       </c>
-      <c r="DE9">
-        <v>0.1</v>
-      </c>
       <c r="DF9">
         <v>0.1</v>
       </c>
-      <c r="DH9">
-        <v>1</v>
-      </c>
-      <c r="DI9" t="s">
-        <v>149</v>
+      <c r="DG9">
+        <v>0.1</v>
+      </c>
+      <c r="DH9" t="s">
+        <v>149</v>
+      </c>
+      <c r="DI9">
+        <v>1</v>
       </c>
       <c r="DJ9" t="s">
         <v>149</v>
@@ -6483,6 +6483,9 @@
       <c r="G10">
         <f>F10-E10</f>
       </c>
+      <c r="H10" t="s">
+        <v>149</v>
+      </c>
       <c r="I10" t="s">
         <v>149</v>
       </c>
@@ -6558,17 +6561,17 @@
       <c r="AG10" t="s">
         <v>149</v>
       </c>
-      <c r="AH10" t="s">
-        <v>149</v>
-      </c>
-      <c r="AI10" t="s">
-        <v>149</v>
-      </c>
-      <c r="AJ10">
-        <v>1</v>
-      </c>
-      <c r="AK10">
-        <v>1</v>
+      <c r="AH10">
+        <v>1</v>
+      </c>
+      <c r="AI10">
+        <v>1</v>
+      </c>
+      <c r="AJ10" t="s">
+        <v>149</v>
+      </c>
+      <c r="AK10" t="s">
+        <v>149</v>
       </c>
       <c r="AL10" t="s">
         <v>149</v>
@@ -6711,9 +6714,6 @@
       <c r="CF10" t="s">
         <v>149</v>
       </c>
-      <c r="CG10" t="s">
-        <v>149</v>
-      </c>
       <c r="CH10" t="s">
         <v>149</v>
       </c>
@@ -6783,10 +6783,10 @@
       <c r="DD10" t="s">
         <v>149</v>
       </c>
-      <c r="DE10" t="s">
-        <v>149</v>
-      </c>
       <c r="DF10" t="s">
+        <v>149</v>
+      </c>
+      <c r="DG10" t="s">
         <v>149</v>
       </c>
       <c r="DH10" t="s">
@@ -6980,14 +6980,14 @@
       <c r="H11" t="s">
         <v>149</v>
       </c>
-      <c r="I11" t="s">
-        <v>149</v>
+      <c r="I11">
+        <v>1</v>
       </c>
       <c r="J11">
         <v>1</v>
       </c>
-      <c r="K11">
-        <v>1</v>
+      <c r="K11" t="s">
+        <v>149</v>
       </c>
       <c r="L11" t="s">
         <v>149</v>
@@ -7040,41 +7040,41 @@
       <c r="AB11" t="s">
         <v>149</v>
       </c>
-      <c r="AC11" t="s">
-        <v>149</v>
+      <c r="AC11">
+        <v>0.5</v>
       </c>
       <c r="AD11" t="s">
         <v>149</v>
       </c>
-      <c r="AE11">
+      <c r="AE11" t="s">
+        <v>149</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>149</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>149</v>
+      </c>
+      <c r="AH11">
         <v>0.5</v>
       </c>
-      <c r="AF11" t="s">
-        <v>149</v>
-      </c>
-      <c r="AG11" t="s">
-        <v>149</v>
-      </c>
-      <c r="AH11" t="s">
-        <v>149</v>
-      </c>
-      <c r="AI11" t="s">
-        <v>149</v>
-      </c>
-      <c r="AJ11">
+      <c r="AI11">
         <v>0.5</v>
       </c>
-      <c r="AK11">
-        <v>0.5</v>
-      </c>
-      <c r="AL11" t="s">
-        <v>149</v>
+      <c r="AJ11" t="s">
+        <v>149</v>
+      </c>
+      <c r="AK11" t="s">
+        <v>149</v>
+      </c>
+      <c r="AL11">
+        <v>1</v>
       </c>
       <c r="AM11" t="s">
         <v>149</v>
       </c>
-      <c r="AN11">
-        <v>1</v>
+      <c r="AN11" t="s">
+        <v>149</v>
       </c>
       <c r="AO11" t="s">
         <v>149</v>
@@ -7289,11 +7289,11 @@
       <c r="DG11" t="s">
         <v>149</v>
       </c>
-      <c r="DH11">
-        <v>1</v>
-      </c>
-      <c r="DI11" t="s">
-        <v>149</v>
+      <c r="DH11" t="s">
+        <v>149</v>
+      </c>
+      <c r="DI11">
+        <v>1</v>
       </c>
       <c r="DJ11" t="s">
         <v>149</v>
@@ -7501,18 +7501,18 @@
       <c r="O12" t="s">
         <v>149</v>
       </c>
-      <c r="P12" t="s">
-        <v>149</v>
-      </c>
-      <c r="Q12">
+      <c r="P12">
         <v>0.5</v>
       </c>
-      <c r="R12" t="s">
-        <v>149</v>
-      </c>
-      <c r="S12">
+      <c r="Q12" t="s">
+        <v>149</v>
+      </c>
+      <c r="R12">
         <v>0.2</v>
       </c>
+      <c r="S12" t="s">
+        <v>149</v>
+      </c>
       <c r="T12" t="s">
         <v>149</v>
       </c>
@@ -7618,14 +7618,14 @@
       <c r="BB12" t="s">
         <v>149</v>
       </c>
-      <c r="BC12" t="s">
-        <v>149</v>
+      <c r="BC12">
+        <v>1</v>
       </c>
       <c r="BD12" t="s">
         <v>149</v>
       </c>
-      <c r="BE12">
-        <v>1</v>
+      <c r="BE12" t="s">
+        <v>149</v>
       </c>
       <c r="BF12" t="s">
         <v>149</v>
@@ -7798,11 +7798,11 @@
       <c r="DJ12" t="s">
         <v>149</v>
       </c>
-      <c r="DK12">
+      <c r="DK12" t="s">
+        <v>149</v>
+      </c>
+      <c r="DL12">
         <v>0.5</v>
-      </c>
-      <c r="DL12" t="s">
-        <v>149</v>
       </c>
       <c r="DM12" t="s">
         <v>149</v>
@@ -8175,29 +8175,29 @@
       <c r="BU13" t="s">
         <v>149</v>
       </c>
-      <c r="BV13" t="s">
-        <v>149</v>
+      <c r="BV13">
+        <v>0.5</v>
       </c>
       <c r="BW13" t="s">
         <v>149</v>
       </c>
-      <c r="BX13">
-        <v>0.5</v>
-      </c>
-      <c r="BY13" t="s">
-        <v>149</v>
+      <c r="BX13" t="s">
+        <v>149</v>
+      </c>
+      <c r="BY13">
+        <v>0.4</v>
       </c>
       <c r="BZ13" t="s">
         <v>149</v>
       </c>
-      <c r="CA13">
-        <v>0.4</v>
+      <c r="CA13" t="s">
+        <v>149</v>
       </c>
       <c r="CB13" t="s">
         <v>149</v>
       </c>
-      <c r="CC13" t="s">
-        <v>149</v>
+      <c r="CC13">
+        <v>1</v>
       </c>
       <c r="CD13" t="s">
         <v>149</v>
@@ -8208,8 +8208,8 @@
       <c r="CF13" t="s">
         <v>149</v>
       </c>
-      <c r="CG13">
-        <v>1</v>
+      <c r="CG13" t="s">
+        <v>149</v>
       </c>
       <c r="CH13" t="s">
         <v>149</v>
@@ -8498,12 +8498,12 @@
       <c r="N14" t="s">
         <v>149</v>
       </c>
-      <c r="O14" t="s">
-        <v>149</v>
-      </c>
-      <c r="P14">
+      <c r="O14">
         <v>0.4</v>
       </c>
+      <c r="P14" t="s">
+        <v>149</v>
+      </c>
       <c r="Q14" t="s">
         <v>149</v>
       </c>
@@ -8561,18 +8561,18 @@
       <c r="AI14" t="s">
         <v>149</v>
       </c>
-      <c r="AJ14" t="s">
-        <v>149</v>
-      </c>
-      <c r="AK14" t="s">
-        <v>149</v>
-      </c>
-      <c r="AL14">
+      <c r="AJ14">
         <v>0.8</v>
       </c>
-      <c r="AM14">
+      <c r="AK14">
         <v>0.8</v>
       </c>
+      <c r="AL14" t="s">
+        <v>149</v>
+      </c>
+      <c r="AM14" t="s">
+        <v>149</v>
+      </c>
       <c r="AN14" t="s">
         <v>149</v>
       </c>
@@ -8651,14 +8651,14 @@
       <c r="BM14" t="s">
         <v>149</v>
       </c>
-      <c r="BN14" t="s">
-        <v>149</v>
+      <c r="BN14">
+        <v>0.6</v>
       </c>
       <c r="BO14" t="s">
         <v>149</v>
       </c>
-      <c r="BP14">
-        <v>0.6</v>
+      <c r="BP14" t="s">
+        <v>149</v>
       </c>
       <c r="BQ14" t="s">
         <v>149</v>
@@ -9061,35 +9061,35 @@
       <c r="AI15" t="s">
         <v>149</v>
       </c>
-      <c r="AJ15" t="s">
-        <v>149</v>
-      </c>
-      <c r="AK15" t="s">
-        <v>149</v>
-      </c>
-      <c r="AL15">
+      <c r="AJ15">
         <v>0.4</v>
       </c>
-      <c r="AM15">
+      <c r="AK15">
         <v>0.4</v>
       </c>
+      <c r="AL15" t="s">
+        <v>149</v>
+      </c>
+      <c r="AM15" t="s">
+        <v>149</v>
+      </c>
       <c r="AN15" t="s">
         <v>149</v>
       </c>
       <c r="AO15" t="s">
         <v>149</v>
       </c>
-      <c r="AP15" t="s">
-        <v>149</v>
-      </c>
-      <c r="AQ15" t="s">
-        <v>149</v>
-      </c>
-      <c r="AR15">
-        <v>1</v>
-      </c>
-      <c r="AS15">
-        <v>1</v>
+      <c r="AP15">
+        <v>1</v>
+      </c>
+      <c r="AQ15">
+        <v>1</v>
+      </c>
+      <c r="AR15" t="s">
+        <v>149</v>
+      </c>
+      <c r="AS15" t="s">
+        <v>149</v>
       </c>
       <c r="AT15" t="s">
         <v>149</v>
@@ -9561,18 +9561,18 @@
       <c r="AI16" t="s">
         <v>149</v>
       </c>
-      <c r="AJ16" t="s">
-        <v>149</v>
-      </c>
-      <c r="AK16" t="s">
-        <v>149</v>
-      </c>
-      <c r="AL16">
+      <c r="AJ16">
         <v>0.4</v>
       </c>
-      <c r="AM16">
+      <c r="AK16">
         <v>0.4</v>
       </c>
+      <c r="AL16" t="s">
+        <v>149</v>
+      </c>
+      <c r="AM16" t="s">
+        <v>149</v>
+      </c>
       <c r="AN16" t="s">
         <v>149</v>
       </c>
@@ -9651,14 +9651,14 @@
       <c r="BM16" t="s">
         <v>149</v>
       </c>
-      <c r="BN16" t="s">
-        <v>149</v>
+      <c r="BN16">
+        <v>0.4</v>
       </c>
       <c r="BO16" t="s">
         <v>149</v>
       </c>
-      <c r="BP16">
-        <v>0.4</v>
+      <c r="BP16" t="s">
+        <v>149</v>
       </c>
       <c r="BQ16" t="s">
         <v>149</v>
@@ -9681,8 +9681,8 @@
       <c r="BW16" t="s">
         <v>149</v>
       </c>
-      <c r="BX16" t="s">
-        <v>149</v>
+      <c r="BX16">
+        <v>1</v>
       </c>
       <c r="BY16" t="s">
         <v>149</v>
@@ -9693,8 +9693,8 @@
       <c r="CA16" t="s">
         <v>149</v>
       </c>
-      <c r="CB16">
-        <v>1</v>
+      <c r="CB16" t="s">
+        <v>149</v>
       </c>
       <c r="CC16" t="s">
         <v>149</v>
@@ -10019,14 +10019,14 @@
       <c r="U17" t="s">
         <v>149</v>
       </c>
-      <c r="V17" t="s">
-        <v>149</v>
-      </c>
-      <c r="W17">
-        <v>1</v>
-      </c>
-      <c r="X17">
-        <v>1</v>
+      <c r="V17">
+        <v>1</v>
+      </c>
+      <c r="W17" t="s">
+        <v>149</v>
+      </c>
+      <c r="X17" t="s">
+        <v>149</v>
       </c>
       <c r="Y17" t="s">
         <v>149</v>
@@ -10136,14 +10136,14 @@
       <c r="BH17" t="s">
         <v>149</v>
       </c>
-      <c r="BI17" t="s">
-        <v>149</v>
+      <c r="BI17">
+        <v>1</v>
       </c>
       <c r="BJ17" t="s">
         <v>149</v>
       </c>
-      <c r="BK17">
-        <v>1</v>
+      <c r="BK17" t="s">
+        <v>149</v>
       </c>
       <c r="BL17" t="s">
         <v>149</v>
@@ -10211,8 +10211,8 @@
       <c r="CG17" t="s">
         <v>149</v>
       </c>
-      <c r="CH17" t="s">
-        <v>149</v>
+      <c r="CH17">
+        <v>1</v>
       </c>
       <c r="CI17" t="s">
         <v>149</v>
@@ -10289,8 +10289,8 @@
       <c r="DG17" t="s">
         <v>149</v>
       </c>
-      <c r="DH17" t="s">
-        <v>149</v>
+      <c r="DH17">
+        <v>1</v>
       </c>
       <c r="DI17" t="s">
         <v>149</v>
@@ -10304,8 +10304,8 @@
       <c r="DL17" t="s">
         <v>149</v>
       </c>
-      <c r="DM17">
-        <v>1</v>
+      <c r="DM17" t="s">
+        <v>149</v>
       </c>
       <c r="DN17">
         <v>1</v>
@@ -10528,14 +10528,14 @@
       <c r="X18" t="s">
         <v>149</v>
       </c>
-      <c r="Y18" t="s">
-        <v>149</v>
+      <c r="Y18">
+        <v>1</v>
       </c>
       <c r="Z18" t="s">
         <v>149</v>
       </c>
-      <c r="AA18">
-        <v>1</v>
+      <c r="AA18" t="s">
+        <v>149</v>
       </c>
       <c r="AB18" t="s">
         <v>149</v>
@@ -11049,17 +11049,17 @@
       <c r="AE19" t="s">
         <v>149</v>
       </c>
-      <c r="AF19" t="s">
-        <v>149</v>
-      </c>
-      <c r="AG19" t="s">
-        <v>149</v>
-      </c>
-      <c r="AH19">
-        <v>1</v>
-      </c>
-      <c r="AI19">
-        <v>1</v>
+      <c r="AF19">
+        <v>1</v>
+      </c>
+      <c r="AG19">
+        <v>1</v>
+      </c>
+      <c r="AH19" t="s">
+        <v>149</v>
+      </c>
+      <c r="AI19" t="s">
+        <v>149</v>
       </c>
       <c r="AJ19" t="s">
         <v>149</v>
@@ -11486,12 +11486,12 @@
       <c r="J20" t="s">
         <v>149</v>
       </c>
-      <c r="K20" t="s">
-        <v>149</v>
-      </c>
-      <c r="L20">
+      <c r="K20">
         <v>0.9</v>
       </c>
+      <c r="L20" t="s">
+        <v>149</v>
+      </c>
       <c r="M20" t="s">
         <v>149</v>
       </c>
@@ -11549,18 +11549,18 @@
       <c r="AE20" t="s">
         <v>149</v>
       </c>
-      <c r="AF20" t="s">
-        <v>149</v>
-      </c>
-      <c r="AG20" t="s">
-        <v>149</v>
-      </c>
-      <c r="AH20">
+      <c r="AF20">
         <v>0.5</v>
       </c>
-      <c r="AI20">
+      <c r="AG20">
         <v>0.5</v>
       </c>
+      <c r="AH20" t="s">
+        <v>149</v>
+      </c>
+      <c r="AI20" t="s">
+        <v>149</v>
+      </c>
       <c r="AJ20" t="s">
         <v>149</v>
       </c>
@@ -11792,11 +11792,11 @@
       <c r="DH20" t="s">
         <v>149</v>
       </c>
-      <c r="DI20">
+      <c r="DI20" t="s">
+        <v>149</v>
+      </c>
+      <c r="DJ20">
         <v>0.9</v>
-      </c>
-      <c r="DJ20" t="s">
-        <v>149</v>
       </c>
       <c r="DK20" t="s">
         <v>149</v>
@@ -12549,18 +12549,18 @@
       <c r="AE22" t="s">
         <v>149</v>
       </c>
-      <c r="AF22" t="s">
-        <v>149</v>
-      </c>
-      <c r="AG22" t="s">
-        <v>149</v>
-      </c>
-      <c r="AH22">
+      <c r="AF22">
         <v>0.5</v>
       </c>
-      <c r="AI22">
+      <c r="AG22">
         <v>0.5</v>
       </c>
+      <c r="AH22" t="s">
+        <v>149</v>
+      </c>
+      <c r="AI22" t="s">
+        <v>149</v>
+      </c>
       <c r="AJ22" t="s">
         <v>149</v>
       </c>
@@ -12585,23 +12585,23 @@
       <c r="AQ22" t="s">
         <v>149</v>
       </c>
-      <c r="AR22" t="s">
-        <v>149</v>
-      </c>
-      <c r="AS22" t="s">
-        <v>149</v>
-      </c>
-      <c r="AT22">
-        <v>1</v>
-      </c>
-      <c r="AU22">
-        <v>1</v>
-      </c>
-      <c r="AV22" t="s">
-        <v>149</v>
-      </c>
-      <c r="AW22" t="s">
-        <v>149</v>
+      <c r="AR22">
+        <v>1</v>
+      </c>
+      <c r="AS22">
+        <v>1</v>
+      </c>
+      <c r="AT22" t="s">
+        <v>149</v>
+      </c>
+      <c r="AU22" t="s">
+        <v>149</v>
+      </c>
+      <c r="AV22">
+        <v>1</v>
+      </c>
+      <c r="AW22">
+        <v>1</v>
       </c>
       <c r="AX22">
         <v>1</v>
@@ -12609,11 +12609,11 @@
       <c r="AY22">
         <v>1</v>
       </c>
-      <c r="AZ22">
-        <v>1</v>
-      </c>
-      <c r="BA22">
-        <v>1</v>
+      <c r="AZ22" t="s">
+        <v>149</v>
+      </c>
+      <c r="BA22" t="s">
+        <v>149</v>
       </c>
       <c r="BB22" t="s">
         <v>149</v>
@@ -13085,35 +13085,35 @@
       <c r="AQ23" t="s">
         <v>149</v>
       </c>
-      <c r="AR23" t="s">
-        <v>149</v>
-      </c>
-      <c r="AS23" t="s">
-        <v>149</v>
-      </c>
-      <c r="AT23">
-        <v>1</v>
-      </c>
-      <c r="AU23">
-        <v>1</v>
-      </c>
-      <c r="AV23" t="s">
-        <v>149</v>
-      </c>
-      <c r="AW23" t="s">
-        <v>149</v>
+      <c r="AR23">
+        <v>1</v>
+      </c>
+      <c r="AS23">
+        <v>1</v>
+      </c>
+      <c r="AT23" t="s">
+        <v>149</v>
+      </c>
+      <c r="AU23" t="s">
+        <v>149</v>
+      </c>
+      <c r="AV23">
+        <v>1</v>
+      </c>
+      <c r="AW23">
+        <v>1</v>
       </c>
       <c r="AX23">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="AY23">
-        <v>1</v>
-      </c>
-      <c r="AZ23">
         <v>0.8</v>
       </c>
-      <c r="BA23">
-        <v>0.8</v>
+      <c r="AZ23" t="s">
+        <v>149</v>
+      </c>
+      <c r="BA23" t="s">
+        <v>149</v>
       </c>
       <c r="BB23" t="s">
         <v>149</v>
@@ -14169,14 +14169,14 @@
       <c r="BS25" t="s">
         <v>149</v>
       </c>
-      <c r="BT25" t="s">
-        <v>149</v>
-      </c>
-      <c r="BU25" t="s">
-        <v>149</v>
-      </c>
-      <c r="BV25">
+      <c r="BT25">
         <v>0.4</v>
+      </c>
+      <c r="BU25">
+        <v>0.4</v>
+      </c>
+      <c r="BV25" t="s">
+        <v>149</v>
       </c>
       <c r="BW25">
         <v>0.4</v>
@@ -14184,8 +14184,8 @@
       <c r="BX25" t="s">
         <v>149</v>
       </c>
-      <c r="BY25">
-        <v>0.4</v>
+      <c r="BY25" t="s">
+        <v>149</v>
       </c>
       <c r="BZ25" t="s">
         <v>149</v>
@@ -14540,17 +14540,17 @@
       <c r="AB26" t="s">
         <v>149</v>
       </c>
-      <c r="AC26" t="s">
-        <v>149</v>
-      </c>
-      <c r="AD26" t="s">
-        <v>149</v>
-      </c>
-      <c r="AE26">
+      <c r="AC26">
         <v>0.5</v>
       </c>
-      <c r="AF26">
-        <v>1</v>
+      <c r="AD26">
+        <v>1</v>
+      </c>
+      <c r="AE26" t="s">
+        <v>149</v>
+      </c>
+      <c r="AF26" t="s">
+        <v>149</v>
       </c>
       <c r="AG26" t="s">
         <v>149</v>
@@ -14666,14 +14666,14 @@
       <c r="BR26" t="s">
         <v>149</v>
       </c>
-      <c r="BS26" t="s">
-        <v>149</v>
+      <c r="BS26">
+        <v>0.6</v>
       </c>
       <c r="BT26" t="s">
         <v>149</v>
       </c>
-      <c r="BU26">
-        <v>0.6</v>
+      <c r="BU26" t="s">
+        <v>149</v>
       </c>
       <c r="BV26" t="s">
         <v>149</v>
@@ -15175,14 +15175,14 @@
       <c r="BU27" t="s">
         <v>149</v>
       </c>
-      <c r="BV27" t="s">
-        <v>149</v>
+      <c r="BV27">
+        <v>0.5</v>
       </c>
       <c r="BW27" t="s">
         <v>149</v>
       </c>
-      <c r="BX27">
-        <v>0.5</v>
+      <c r="BX27" t="s">
+        <v>149</v>
       </c>
       <c r="BY27" t="s">
         <v>149</v>
@@ -15190,23 +15190,23 @@
       <c r="BZ27" t="s">
         <v>149</v>
       </c>
-      <c r="CA27" t="s">
-        <v>149</v>
+      <c r="CA27">
+        <v>1</v>
       </c>
       <c r="CB27" t="s">
         <v>149</v>
       </c>
-      <c r="CC27">
-        <v>1</v>
-      </c>
-      <c r="CD27" t="s">
-        <v>149</v>
+      <c r="CC27" t="s">
+        <v>149</v>
+      </c>
+      <c r="CD27">
+        <v>1</v>
       </c>
       <c r="CE27" t="s">
         <v>149</v>
       </c>
-      <c r="CF27">
-        <v>1</v>
+      <c r="CF27" t="s">
+        <v>149</v>
       </c>
       <c r="CG27" t="s">
         <v>149</v>
@@ -15477,12 +15477,12 @@
       <c r="G28">
         <f>F28-E28</f>
       </c>
-      <c r="H28" t="s">
-        <v>149</v>
-      </c>
-      <c r="I28">
+      <c r="H28">
         <v>0.6</v>
       </c>
+      <c r="I28" t="s">
+        <v>149</v>
+      </c>
       <c r="J28" t="s">
         <v>149</v>
       </c>
@@ -15504,12 +15504,12 @@
       <c r="P28" t="s">
         <v>149</v>
       </c>
-      <c r="Q28" t="s">
-        <v>149</v>
-      </c>
-      <c r="R28">
+      <c r="Q28">
         <v>0.2</v>
       </c>
+      <c r="R28" t="s">
+        <v>149</v>
+      </c>
       <c r="S28" t="s">
         <v>149</v>
       </c>
@@ -15780,14 +15780,14 @@
       <c r="DD28" t="s">
         <v>149</v>
       </c>
-      <c r="DE28">
-        <v>0.6</v>
+      <c r="DE28" t="s">
+        <v>149</v>
       </c>
       <c r="DF28">
         <v>0.6</v>
       </c>
-      <c r="DG28" t="s">
-        <v>149</v>
+      <c r="DG28">
+        <v>0.6</v>
       </c>
       <c r="DH28" t="s">
         <v>149</v>
@@ -15977,12 +15977,12 @@
       <c r="G29">
         <f>F29-E29</f>
       </c>
-      <c r="H29" t="s">
-        <v>149</v>
-      </c>
-      <c r="I29">
+      <c r="H29">
         <v>0.5</v>
       </c>
+      <c r="I29" t="s">
+        <v>149</v>
+      </c>
       <c r="J29" t="s">
         <v>149</v>
       </c>
@@ -16016,12 +16016,12 @@
       <c r="T29" t="s">
         <v>149</v>
       </c>
-      <c r="U29" t="s">
-        <v>149</v>
-      </c>
-      <c r="V29">
+      <c r="U29">
         <v>0.4</v>
       </c>
+      <c r="V29" t="s">
+        <v>149</v>
+      </c>
       <c r="W29" t="s">
         <v>149</v>
       </c>
@@ -16130,14 +16130,14 @@
       <c r="BF29" t="s">
         <v>149</v>
       </c>
-      <c r="BG29" t="s">
-        <v>149</v>
+      <c r="BG29">
+        <v>1</v>
       </c>
       <c r="BH29" t="s">
         <v>149</v>
       </c>
-      <c r="BI29">
-        <v>1</v>
+      <c r="BI29" t="s">
+        <v>149</v>
       </c>
       <c r="BJ29" t="s">
         <v>149</v>
@@ -16145,14 +16145,14 @@
       <c r="BK29" t="s">
         <v>149</v>
       </c>
-      <c r="BL29" t="s">
-        <v>149</v>
+      <c r="BL29">
+        <v>1</v>
       </c>
       <c r="BM29" t="s">
         <v>149</v>
       </c>
-      <c r="BN29">
-        <v>1</v>
+      <c r="BN29" t="s">
+        <v>149</v>
       </c>
       <c r="BO29" t="s">
         <v>149</v>
@@ -16280,14 +16280,14 @@
       <c r="DD29" t="s">
         <v>149</v>
       </c>
-      <c r="DE29">
-        <v>0.5</v>
+      <c r="DE29" t="s">
+        <v>149</v>
       </c>
       <c r="DF29">
         <v>0.5</v>
       </c>
-      <c r="DG29" t="s">
-        <v>149</v>
+      <c r="DG29">
+        <v>0.5</v>
       </c>
       <c r="DH29" t="s">
         <v>149</v>
@@ -16507,12 +16507,12 @@
       <c r="Q30" t="s">
         <v>149</v>
       </c>
-      <c r="R30" t="s">
-        <v>149</v>
-      </c>
-      <c r="S30">
+      <c r="R30">
         <v>0.5</v>
       </c>
+      <c r="S30" t="s">
+        <v>149</v>
+      </c>
       <c r="T30" t="s">
         <v>149</v>
       </c>
@@ -16534,14 +16534,14 @@
       <c r="Z30" t="s">
         <v>149</v>
       </c>
-      <c r="AA30" t="s">
-        <v>149</v>
+      <c r="AA30">
+        <v>0.6</v>
       </c>
       <c r="AB30" t="s">
         <v>149</v>
       </c>
-      <c r="AC30">
-        <v>0.6</v>
+      <c r="AC30" t="s">
+        <v>149</v>
       </c>
       <c r="AD30" t="s">
         <v>149</v>
@@ -16591,29 +16591,29 @@
       <c r="AS30" t="s">
         <v>149</v>
       </c>
-      <c r="AT30" t="s">
-        <v>149</v>
-      </c>
-      <c r="AU30" t="s">
-        <v>149</v>
-      </c>
-      <c r="AV30">
+      <c r="AT30">
         <v>0.5</v>
       </c>
-      <c r="AW30">
+      <c r="AU30">
         <v>0.5</v>
       </c>
-      <c r="AX30" t="s">
-        <v>149</v>
-      </c>
-      <c r="AY30" t="s">
-        <v>149</v>
-      </c>
-      <c r="AZ30">
+      <c r="AV30" t="s">
+        <v>149</v>
+      </c>
+      <c r="AW30" t="s">
+        <v>149</v>
+      </c>
+      <c r="AX30">
         <v>0.2</v>
       </c>
-      <c r="BA30">
+      <c r="AY30">
         <v>0.2</v>
+      </c>
+      <c r="AZ30" t="s">
+        <v>149</v>
+      </c>
+      <c r="BA30" t="s">
+        <v>149</v>
       </c>
       <c r="BB30" t="s">
         <v>149</v>
@@ -17073,14 +17073,14 @@
       <c r="AM31" t="s">
         <v>149</v>
       </c>
-      <c r="AN31" t="s">
-        <v>149</v>
+      <c r="AN31">
+        <v>0.6</v>
       </c>
       <c r="AO31" t="s">
         <v>149</v>
       </c>
-      <c r="AP31">
-        <v>0.6</v>
+      <c r="AP31" t="s">
+        <v>149</v>
       </c>
       <c r="AQ31" t="s">
         <v>149</v>
@@ -17091,18 +17091,18 @@
       <c r="AS31" t="s">
         <v>149</v>
       </c>
-      <c r="AT31" t="s">
-        <v>149</v>
-      </c>
-      <c r="AU31" t="s">
-        <v>149</v>
-      </c>
-      <c r="AV31">
+      <c r="AT31">
         <v>0.5</v>
       </c>
-      <c r="AW31">
+      <c r="AU31">
         <v>0.5</v>
       </c>
+      <c r="AV31" t="s">
+        <v>149</v>
+      </c>
+      <c r="AW31" t="s">
+        <v>149</v>
+      </c>
       <c r="AX31" t="s">
         <v>149</v>
       </c>
@@ -17133,14 +17133,14 @@
       <c r="BG31" t="s">
         <v>149</v>
       </c>
-      <c r="BH31" t="s">
-        <v>149</v>
+      <c r="BH31">
+        <v>1</v>
       </c>
       <c r="BI31" t="s">
         <v>149</v>
       </c>
-      <c r="BJ31">
-        <v>1</v>
+      <c r="BJ31" t="s">
+        <v>149</v>
       </c>
       <c r="BK31" t="s">
         <v>149</v>
@@ -17154,17 +17154,17 @@
       <c r="BN31" t="s">
         <v>149</v>
       </c>
-      <c r="BO31" t="s">
-        <v>149</v>
-      </c>
-      <c r="BP31" t="s">
-        <v>149</v>
-      </c>
-      <c r="BQ31">
-        <v>1</v>
-      </c>
-      <c r="BR31">
-        <v>1</v>
+      <c r="BO31">
+        <v>1</v>
+      </c>
+      <c r="BP31">
+        <v>1</v>
+      </c>
+      <c r="BQ31" t="s">
+        <v>149</v>
+      </c>
+      <c r="BR31" t="s">
+        <v>149</v>
       </c>
       <c r="BS31" t="s">
         <v>149</v>
@@ -17525,14 +17525,14 @@
       <c r="W32" t="s">
         <v>149</v>
       </c>
-      <c r="X32" t="s">
-        <v>149</v>
+      <c r="X32">
+        <v>1</v>
       </c>
       <c r="Y32" t="s">
         <v>149</v>
       </c>
-      <c r="Z32">
-        <v>1</v>
+      <c r="Z32" t="s">
+        <v>149</v>
       </c>
       <c r="AA32" t="s">
         <v>149</v>
@@ -17648,8 +17648,8 @@
       <c r="BL32" t="s">
         <v>149</v>
       </c>
-      <c r="BM32" t="s">
-        <v>149</v>
+      <c r="BM32">
+        <v>1</v>
       </c>
       <c r="BN32" t="s">
         <v>149</v>
@@ -17657,14 +17657,14 @@
       <c r="BO32">
         <v>1</v>
       </c>
-      <c r="BP32" t="s">
-        <v>149</v>
-      </c>
-      <c r="BQ32">
-        <v>1</v>
-      </c>
-      <c r="BR32">
-        <v>1</v>
+      <c r="BP32">
+        <v>1</v>
+      </c>
+      <c r="BQ32" t="s">
+        <v>149</v>
+      </c>
+      <c r="BR32" t="s">
+        <v>149</v>
       </c>
       <c r="BS32" t="s">
         <v>149</v>
@@ -17977,12 +17977,12 @@
       <c r="G33">
         <f>F33-E33</f>
       </c>
-      <c r="H33" t="s">
-        <v>149</v>
-      </c>
-      <c r="I33">
+      <c r="H33">
         <v>0.5</v>
       </c>
+      <c r="I33" t="s">
+        <v>149</v>
+      </c>
       <c r="J33" t="s">
         <v>149</v>
       </c>
@@ -18013,11 +18013,11 @@
       <c r="S33" t="s">
         <v>149</v>
       </c>
-      <c r="T33" t="s">
-        <v>149</v>
-      </c>
-      <c r="U33">
-        <v>1</v>
+      <c r="T33">
+        <v>1</v>
+      </c>
+      <c r="U33" t="s">
+        <v>149</v>
       </c>
       <c r="V33" t="s">
         <v>149</v>
@@ -18073,17 +18073,17 @@
       <c r="AM33" t="s">
         <v>149</v>
       </c>
-      <c r="AN33" t="s">
-        <v>149</v>
-      </c>
-      <c r="AO33" t="s">
-        <v>149</v>
-      </c>
-      <c r="AP33">
+      <c r="AN33">
         <v>0.4</v>
       </c>
-      <c r="AQ33">
-        <v>1</v>
+      <c r="AO33">
+        <v>1</v>
+      </c>
+      <c r="AP33" t="s">
+        <v>149</v>
+      </c>
+      <c r="AQ33" t="s">
+        <v>149</v>
       </c>
       <c r="AR33" t="s">
         <v>149</v>
@@ -18280,14 +18280,14 @@
       <c r="DD33" t="s">
         <v>149</v>
       </c>
-      <c r="DE33">
-        <v>0.5</v>
+      <c r="DE33" t="s">
+        <v>149</v>
       </c>
       <c r="DF33">
         <v>0.5</v>
       </c>
-      <c r="DG33" t="s">
-        <v>149</v>
+      <c r="DG33">
+        <v>0.5</v>
       </c>
       <c r="DH33" t="s">
         <v>149</v>
@@ -18495,12 +18495,12 @@
       <c r="M34" t="s">
         <v>149</v>
       </c>
-      <c r="N34" t="s">
-        <v>149</v>
-      </c>
-      <c r="O34">
+      <c r="N34">
         <v>0.5</v>
       </c>
+      <c r="O34" t="s">
+        <v>149</v>
+      </c>
       <c r="P34" t="s">
         <v>149</v>
       </c>
@@ -18531,14 +18531,14 @@
       <c r="Y34" t="s">
         <v>149</v>
       </c>
-      <c r="Z34" t="s">
-        <v>149</v>
+      <c r="Z34">
+        <v>1</v>
       </c>
       <c r="AA34" t="s">
         <v>149</v>
       </c>
-      <c r="AB34">
-        <v>1</v>
+      <c r="AB34" t="s">
+        <v>149</v>
       </c>
       <c r="AC34" t="s">
         <v>149</v>
@@ -19109,17 +19109,17 @@
       <c r="AY35" t="s">
         <v>149</v>
       </c>
-      <c r="AZ35" t="s">
-        <v>149</v>
-      </c>
-      <c r="BA35" t="s">
-        <v>149</v>
-      </c>
-      <c r="BB35">
-        <v>1</v>
-      </c>
-      <c r="BC35">
-        <v>1</v>
+      <c r="AZ35">
+        <v>1</v>
+      </c>
+      <c r="BA35">
+        <v>1</v>
+      </c>
+      <c r="BB35" t="s">
+        <v>149</v>
+      </c>
+      <c r="BC35" t="s">
+        <v>149</v>
       </c>
       <c r="BD35" t="s">
         <v>149</v>
@@ -19142,14 +19142,14 @@
       <c r="BJ35" t="s">
         <v>149</v>
       </c>
-      <c r="BK35" t="s">
-        <v>149</v>
+      <c r="BK35">
+        <v>1</v>
       </c>
       <c r="BL35" t="s">
         <v>149</v>
       </c>
-      <c r="BM35">
-        <v>1</v>
+      <c r="BM35" t="s">
+        <v>149</v>
       </c>
       <c r="BN35" t="s">
         <v>149</v>
@@ -19498,12 +19498,12 @@
       <c r="N36" t="s">
         <v>149</v>
       </c>
-      <c r="O36" t="s">
-        <v>149</v>
-      </c>
-      <c r="P36">
+      <c r="O36">
         <v>0.6</v>
       </c>
+      <c r="P36" t="s">
+        <v>149</v>
+      </c>
       <c r="Q36" t="s">
         <v>149</v>
       </c>
@@ -19639,14 +19639,14 @@
       <c r="BI36" t="s">
         <v>149</v>
       </c>
-      <c r="BJ36" t="s">
-        <v>149</v>
+      <c r="BJ36">
+        <v>0.4</v>
       </c>
       <c r="BK36" t="s">
         <v>149</v>
       </c>
-      <c r="BL36">
-        <v>0.4</v>
+      <c r="BL36" t="s">
+        <v>149</v>
       </c>
       <c r="BM36" t="s">
         <v>149</v>
@@ -19986,12 +19986,12 @@
       <c r="J37" t="s">
         <v>149</v>
       </c>
-      <c r="K37" t="s">
-        <v>149</v>
-      </c>
-      <c r="L37">
+      <c r="K37">
         <v>0.2</v>
       </c>
+      <c r="L37" t="s">
+        <v>149</v>
+      </c>
       <c r="M37" t="s">
         <v>149</v>
       </c>
@@ -20037,14 +20037,14 @@
       <c r="AA37" t="s">
         <v>149</v>
       </c>
-      <c r="AB37" t="s">
-        <v>149</v>
+      <c r="AB37">
+        <v>1</v>
       </c>
       <c r="AC37" t="s">
         <v>149</v>
       </c>
-      <c r="AD37">
-        <v>1</v>
+      <c r="AD37" t="s">
+        <v>149</v>
       </c>
       <c r="AE37" t="s">
         <v>149</v>
@@ -20091,18 +20091,18 @@
       <c r="AS37" t="s">
         <v>149</v>
       </c>
-      <c r="AT37" t="s">
-        <v>149</v>
-      </c>
-      <c r="AU37" t="s">
-        <v>149</v>
-      </c>
-      <c r="AV37">
+      <c r="AT37">
         <v>0.5</v>
       </c>
-      <c r="AW37">
+      <c r="AU37">
         <v>0.5</v>
       </c>
+      <c r="AV37" t="s">
+        <v>149</v>
+      </c>
+      <c r="AW37" t="s">
+        <v>149</v>
+      </c>
       <c r="AX37" t="s">
         <v>149</v>
       </c>
@@ -20121,20 +20121,20 @@
       <c r="BC37" t="s">
         <v>149</v>
       </c>
-      <c r="BD37" t="s">
-        <v>149</v>
+      <c r="BD37">
+        <v>0.5</v>
       </c>
       <c r="BE37" t="s">
         <v>149</v>
       </c>
       <c r="BF37">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="BG37" t="s">
         <v>149</v>
       </c>
-      <c r="BH37">
-        <v>0.7</v>
+      <c r="BH37" t="s">
+        <v>149</v>
       </c>
       <c r="BI37" t="s">
         <v>149</v>
@@ -20292,11 +20292,11 @@
       <c r="DH37" t="s">
         <v>149</v>
       </c>
-      <c r="DI37">
+      <c r="DI37" t="s">
+        <v>149</v>
+      </c>
+      <c r="DJ37">
         <v>0.2</v>
-      </c>
-      <c r="DJ37" t="s">
-        <v>149</v>
       </c>
       <c r="DK37" t="s">
         <v>149</v>
@@ -20516,11 +20516,11 @@
       <c r="T38" t="s">
         <v>149</v>
       </c>
-      <c r="U38" t="s">
-        <v>149</v>
-      </c>
-      <c r="V38">
-        <v>1</v>
+      <c r="U38">
+        <v>1</v>
+      </c>
+      <c r="V38" t="s">
+        <v>149</v>
       </c>
       <c r="W38" t="s">
         <v>149</v>
@@ -20591,18 +20591,18 @@
       <c r="AS38" t="s">
         <v>149</v>
       </c>
-      <c r="AT38" t="s">
-        <v>149</v>
-      </c>
-      <c r="AU38" t="s">
-        <v>149</v>
-      </c>
-      <c r="AV38">
+      <c r="AT38">
         <v>0.5</v>
       </c>
-      <c r="AW38">
+      <c r="AU38">
         <v>0.5</v>
       </c>
+      <c r="AV38" t="s">
+        <v>149</v>
+      </c>
+      <c r="AW38" t="s">
+        <v>149</v>
+      </c>
       <c r="AX38" t="s">
         <v>149</v>
       </c>
@@ -20627,26 +20627,26 @@
       <c r="BE38" t="s">
         <v>149</v>
       </c>
-      <c r="BF38" t="s">
-        <v>149</v>
+      <c r="BF38">
+        <v>0.3</v>
       </c>
       <c r="BG38" t="s">
         <v>149</v>
       </c>
-      <c r="BH38">
-        <v>0.3</v>
+      <c r="BH38" t="s">
+        <v>149</v>
       </c>
       <c r="BI38" t="s">
         <v>149</v>
       </c>
-      <c r="BJ38" t="s">
-        <v>149</v>
+      <c r="BJ38">
+        <v>0.6</v>
       </c>
       <c r="BK38" t="s">
         <v>149</v>
       </c>
-      <c r="BL38">
-        <v>0.6</v>
+      <c r="BL38" t="s">
+        <v>149</v>
       </c>
       <c r="BM38" t="s">
         <v>149</v>
@@ -20992,11 +20992,11 @@
       <c r="L39" t="s">
         <v>149</v>
       </c>
-      <c r="M39" t="s">
-        <v>149</v>
-      </c>
-      <c r="N39">
-        <v>1</v>
+      <c r="M39">
+        <v>1</v>
+      </c>
+      <c r="N39" t="s">
+        <v>149</v>
       </c>
       <c r="O39" t="s">
         <v>149</v>
@@ -21160,17 +21160,17 @@
       <c r="BP39" t="s">
         <v>149</v>
       </c>
-      <c r="BQ39" t="s">
-        <v>149</v>
-      </c>
-      <c r="BR39" t="s">
-        <v>149</v>
-      </c>
-      <c r="BS39">
-        <v>1</v>
-      </c>
-      <c r="BT39">
-        <v>1</v>
+      <c r="BQ39">
+        <v>1</v>
+      </c>
+      <c r="BR39">
+        <v>1</v>
+      </c>
+      <c r="BS39" t="s">
+        <v>149</v>
+      </c>
+      <c r="BT39" t="s">
+        <v>149</v>
       </c>
       <c r="BU39" t="s">
         <v>149</v>
@@ -21295,11 +21295,11 @@
       <c r="DI39" t="s">
         <v>149</v>
       </c>
-      <c r="DJ39">
-        <v>1</v>
-      </c>
-      <c r="DK39" t="s">
-        <v>149</v>
+      <c r="DJ39" t="s">
+        <v>149</v>
+      </c>
+      <c r="DK39">
+        <v>1</v>
       </c>
       <c r="DL39" t="s">
         <v>149</v>
@@ -21495,12 +21495,12 @@
       <c r="M40" t="s">
         <v>149</v>
       </c>
-      <c r="N40" t="s">
-        <v>149</v>
-      </c>
-      <c r="O40">
+      <c r="N40">
         <v>0.5</v>
       </c>
+      <c r="O40" t="s">
+        <v>149</v>
+      </c>
       <c r="P40" t="s">
         <v>149</v>
       </c>
@@ -21555,18 +21555,18 @@
       <c r="AG40" t="s">
         <v>149</v>
       </c>
-      <c r="AH40" t="s">
-        <v>149</v>
-      </c>
-      <c r="AI40" t="s">
-        <v>149</v>
-      </c>
-      <c r="AJ40">
+      <c r="AH40">
         <v>0.5</v>
       </c>
-      <c r="AK40">
+      <c r="AI40">
         <v>0.5</v>
       </c>
+      <c r="AJ40" t="s">
+        <v>149</v>
+      </c>
+      <c r="AK40" t="s">
+        <v>149</v>
+      </c>
       <c r="AL40" t="s">
         <v>149</v>
       </c>
@@ -21660,17 +21660,17 @@
       <c r="BP40" t="s">
         <v>149</v>
       </c>
-      <c r="BQ40" t="s">
-        <v>149</v>
-      </c>
-      <c r="BR40" t="s">
-        <v>149</v>
-      </c>
-      <c r="BS40">
-        <v>1</v>
-      </c>
-      <c r="BT40">
-        <v>1</v>
+      <c r="BQ40">
+        <v>1</v>
+      </c>
+      <c r="BR40">
+        <v>1</v>
+      </c>
+      <c r="BS40" t="s">
+        <v>149</v>
+      </c>
+      <c r="BT40" t="s">
+        <v>149</v>
       </c>
       <c r="BU40" t="s">
         <v>149</v>
@@ -21684,14 +21684,14 @@
       <c r="BX40" t="s">
         <v>149</v>
       </c>
-      <c r="BY40" t="s">
-        <v>149</v>
+      <c r="BY40">
+        <v>0.6</v>
       </c>
       <c r="BZ40" t="s">
         <v>149</v>
       </c>
-      <c r="CA40">
-        <v>0.6</v>
+      <c r="CA40" t="s">
+        <v>149</v>
       </c>
       <c r="CB40" t="s">
         <v>149</v>
@@ -21977,12 +21977,12 @@
       <c r="G41">
         <f>F41-E41</f>
       </c>
-      <c r="H41" t="s">
-        <v>149</v>
-      </c>
-      <c r="I41">
+      <c r="H41">
         <v>0.4</v>
       </c>
+      <c r="I41" t="s">
+        <v>149</v>
+      </c>
       <c r="J41" t="s">
         <v>149</v>
       </c>
@@ -22172,14 +22172,14 @@
       <c r="BT41" t="s">
         <v>149</v>
       </c>
-      <c r="BU41" t="s">
-        <v>149</v>
+      <c r="BU41">
+        <v>0.2</v>
       </c>
       <c r="BV41" t="s">
         <v>149</v>
       </c>
-      <c r="BW41">
-        <v>0.2</v>
+      <c r="BW41" t="s">
+        <v>149</v>
       </c>
       <c r="BX41" t="s">
         <v>149</v>
@@ -22193,14 +22193,14 @@
       <c r="CA41" t="s">
         <v>149</v>
       </c>
-      <c r="CB41" t="s">
-        <v>149</v>
+      <c r="CB41">
+        <v>1</v>
       </c>
       <c r="CC41" t="s">
         <v>149</v>
       </c>
-      <c r="CD41">
-        <v>1</v>
+      <c r="CD41" t="s">
+        <v>149</v>
       </c>
       <c r="CE41" t="s">
         <v>149</v>
@@ -22280,14 +22280,14 @@
       <c r="DD41" t="s">
         <v>149</v>
       </c>
-      <c r="DE41">
-        <v>0.4</v>
+      <c r="DE41" t="s">
+        <v>149</v>
       </c>
       <c r="DF41">
         <v>0.4</v>
       </c>
-      <c r="DG41" t="s">
-        <v>149</v>
+      <c r="DG41">
+        <v>0.4</v>
       </c>
       <c r="DH41" t="s">
         <v>149</v>
@@ -22489,12 +22489,12 @@
       <c r="K42" t="s">
         <v>149</v>
       </c>
-      <c r="L42" t="s">
-        <v>149</v>
-      </c>
-      <c r="M42">
+      <c r="L42">
         <v>0.4</v>
       </c>
+      <c r="M42" t="s">
+        <v>149</v>
+      </c>
       <c r="N42" t="s">
         <v>149</v>
       </c>
@@ -22510,12 +22510,12 @@
       <c r="R42" t="s">
         <v>149</v>
       </c>
-      <c r="S42" t="s">
-        <v>149</v>
-      </c>
-      <c r="T42">
+      <c r="S42">
         <v>0.5</v>
       </c>
+      <c r="T42" t="s">
+        <v>149</v>
+      </c>
       <c r="U42" t="s">
         <v>149</v>
       </c>
@@ -22621,17 +22621,17 @@
       <c r="BC42" t="s">
         <v>149</v>
       </c>
-      <c r="BD42" t="s">
-        <v>149</v>
-      </c>
-      <c r="BE42" t="s">
-        <v>149</v>
-      </c>
-      <c r="BF42">
+      <c r="BD42">
         <v>0.7</v>
       </c>
-      <c r="BG42">
+      <c r="BE42">
         <v>0.6</v>
+      </c>
+      <c r="BF42" t="s">
+        <v>149</v>
+      </c>
+      <c r="BG42" t="s">
+        <v>149</v>
       </c>
       <c r="BH42" t="s">
         <v>149</v>
@@ -22801,11 +22801,11 @@
       <c r="DK42" t="s">
         <v>149</v>
       </c>
-      <c r="DL42">
+      <c r="DL42" t="s">
+        <v>149</v>
+      </c>
+      <c r="DM42">
         <v>0.5</v>
-      </c>
-      <c r="DM42" t="s">
-        <v>149</v>
       </c>
       <c r="DN42" t="s">
         <v>149</v>
@@ -23007,11 +23007,11 @@
       <c r="Q43" t="s">
         <v>149</v>
       </c>
-      <c r="R43" t="s">
-        <v>149</v>
-      </c>
-      <c r="S43">
+      <c r="R43">
         <v>0.4</v>
+      </c>
+      <c r="S43" t="s">
+        <v>149</v>
       </c>
       <c r="T43" t="s">
         <v>149</v>
@@ -23669,23 +23669,23 @@
       <c r="BS44" t="s">
         <v>149</v>
       </c>
-      <c r="BT44" t="s">
-        <v>149</v>
-      </c>
-      <c r="BU44" t="s">
-        <v>149</v>
-      </c>
-      <c r="BV44">
+      <c r="BT44">
         <v>0.6</v>
       </c>
+      <c r="BU44">
+        <v>0.4</v>
+      </c>
+      <c r="BV44" t="s">
+        <v>149</v>
+      </c>
       <c r="BW44">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="BX44" t="s">
         <v>149</v>
       </c>
-      <c r="BY44">
-        <v>0.6</v>
+      <c r="BY44" t="s">
+        <v>149</v>
       </c>
       <c r="BZ44" t="s">
         <v>149</v>
@@ -24007,12 +24007,12 @@
       <c r="Q45" t="s">
         <v>149</v>
       </c>
-      <c r="R45" t="s">
-        <v>149</v>
-      </c>
-      <c r="S45">
+      <c r="R45">
         <v>0.5</v>
       </c>
+      <c r="S45" t="s">
+        <v>149</v>
+      </c>
       <c r="T45" t="s">
         <v>149</v>
       </c>
@@ -24034,14 +24034,14 @@
       <c r="Z45" t="s">
         <v>149</v>
       </c>
-      <c r="AA45" t="s">
-        <v>149</v>
+      <c r="AA45">
+        <v>0.4</v>
       </c>
       <c r="AB45" t="s">
         <v>149</v>
       </c>
-      <c r="AC45">
-        <v>0.4</v>
+      <c r="AC45" t="s">
+        <v>149</v>
       </c>
       <c r="AD45" t="s">
         <v>149</v>
@@ -24489,12 +24489,12 @@
       <c r="K46" t="s">
         <v>149</v>
       </c>
-      <c r="L46" t="s">
-        <v>149</v>
-      </c>
-      <c r="M46">
+      <c r="L46">
         <v>0.7</v>
       </c>
+      <c r="M46" t="s">
+        <v>149</v>
+      </c>
       <c r="N46" t="s">
         <v>149</v>
       </c>
@@ -24510,12 +24510,12 @@
       <c r="R46" t="s">
         <v>149</v>
       </c>
-      <c r="S46" t="s">
-        <v>149</v>
-      </c>
-      <c r="T46">
+      <c r="S46">
         <v>0.4</v>
       </c>
+      <c r="T46" t="s">
+        <v>149</v>
+      </c>
       <c r="U46" t="s">
         <v>149</v>
       </c>
@@ -24801,11 +24801,11 @@
       <c r="DK46" t="s">
         <v>149</v>
       </c>
-      <c r="DL46">
+      <c r="DL46" t="s">
+        <v>149</v>
+      </c>
+      <c r="DM46">
         <v>0.4</v>
-      </c>
-      <c r="DM46" t="s">
-        <v>149</v>
       </c>
       <c r="DN46" t="s">
         <v>149</v>
@@ -24980,14 +24980,14 @@
       <c r="H47" t="s">
         <v>149</v>
       </c>
-      <c r="I47" t="s">
-        <v>149</v>
+      <c r="I47">
+        <v>1</v>
       </c>
       <c r="J47">
         <v>1</v>
       </c>
-      <c r="K47">
-        <v>1</v>
+      <c r="K47" t="s">
+        <v>149</v>
       </c>
       <c r="L47" t="s">
         <v>149</v>
@@ -25289,11 +25289,11 @@
       <c r="DG47" t="s">
         <v>149</v>
       </c>
-      <c r="DH47">
-        <v>1</v>
-      </c>
-      <c r="DI47" t="s">
-        <v>149</v>
+      <c r="DH47" t="s">
+        <v>149</v>
+      </c>
+      <c r="DI47">
+        <v>1</v>
       </c>
       <c r="DJ47" t="s">
         <v>149</v>
@@ -25621,17 +25621,17 @@
       <c r="BC48" t="s">
         <v>149</v>
       </c>
-      <c r="BD48" t="s">
-        <v>149</v>
-      </c>
-      <c r="BE48" t="s">
-        <v>149</v>
-      </c>
-      <c r="BF48">
+      <c r="BD48">
         <v>0.3</v>
       </c>
-      <c r="BG48">
+      <c r="BE48">
         <v>0.4</v>
+      </c>
+      <c r="BF48" t="s">
+        <v>149</v>
+      </c>
+      <c r="BG48" t="s">
+        <v>149</v>
       </c>
       <c r="BH48" t="s">
         <v>149</v>
@@ -25962,7 +25962,10 @@
       <c r="H49" t="s">
         <v>149</v>
       </c>
-      <c r="I49" t="s">
+      <c r="AF49" t="s">
+        <v>149</v>
+      </c>
+      <c r="AG49" t="s">
         <v>149</v>
       </c>
       <c r="AH49" t="s">
@@ -25971,18 +25974,18 @@
       <c r="AI49" t="s">
         <v>149</v>
       </c>
-      <c r="AJ49" t="s">
-        <v>149</v>
-      </c>
-      <c r="AK49" t="s">
-        <v>149</v>
-      </c>
-      <c r="AL49">
+      <c r="AJ49">
         <v>0.3</v>
       </c>
-      <c r="AM49">
+      <c r="AK49">
         <v>0.3</v>
       </c>
+      <c r="AR49" t="s">
+        <v>149</v>
+      </c>
+      <c r="AS49" t="s">
+        <v>149</v>
+      </c>
       <c r="AT49" t="s">
         <v>149</v>
       </c>
@@ -26001,10 +26004,10 @@
       <c r="AY49" t="s">
         <v>149</v>
       </c>
-      <c r="AZ49" t="s">
-        <v>149</v>
-      </c>
-      <c r="BA49" t="s">
+      <c r="BO49" t="s">
+        <v>149</v>
+      </c>
+      <c r="BP49" t="s">
         <v>149</v>
       </c>
       <c r="BQ49" t="s">
@@ -26013,10 +26016,7 @@
       <c r="BR49" t="s">
         <v>149</v>
       </c>
-      <c r="BS49" t="s">
-        <v>149</v>
-      </c>
-      <c r="BT49" t="s">
+      <c r="CG49" t="s">
         <v>149</v>
       </c>
       <c r="CO49" t="s">
@@ -26096,10 +26096,10 @@
       <c r="D50">
         <f>SUM(D9:D49)</f>
       </c>
-      <c r="AV50" t="s">
-        <v>149</v>
-      </c>
-      <c r="AW50" t="s">
+      <c r="AT50" t="s">
+        <v>149</v>
+      </c>
+      <c r="AU50" t="s">
         <v>149</v>
       </c>
       <c r="CS50" t="s">

</xml_diff>